<commit_message>
Removing CO allocation from spreadsheet template
</commit_message>
<xml_diff>
--- a/spec/support/allocationDuplicateRo.xlsx
+++ b/spec/support/allocationDuplicateRo.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="125">
   <si>
     <t>Example</t>
   </si>
@@ -385,9 +385,6 @@
   </si>
   <si>
     <t>Number of Hearing Days Allocated in Date Range</t>
-  </si>
-  <si>
-    <t>Central Office</t>
   </si>
   <si>
     <t xml:space="preserve">Des Moines, IA </t>
@@ -532,7 +529,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -911,49 +908,6 @@
         <color indexed="12"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
@@ -971,7 +925,9 @@
       <right style="thin">
         <color indexed="8"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -998,6 +954,17 @@
         <color indexed="8"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="12"/>
       </bottom>
@@ -1009,7 +976,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1199,40 +1166,37 @@
     <xf numFmtId="49" fontId="9" fillId="4" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="8" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -6316,7 +6280,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N101"/>
+  <dimension ref="A1:N100"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -6403,14 +6367,16 @@
       <c r="M3" s="31"/>
       <c r="N3" s="31"/>
     </row>
-    <row r="4" ht="30.95" customHeight="1">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="65"/>
       <c r="B4" t="s" s="66">
-        <v>124</v>
-      </c>
-      <c r="C4" s="67"/>
+        <v>63</v>
+      </c>
+      <c r="C4" t="s" s="67">
+        <v>4</v>
+      </c>
       <c r="D4" s="68">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" s="46"/>
       <c r="F4" s="31"/>
@@ -6426,13 +6392,13 @@
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="69"/>
       <c r="B5" t="s" s="66">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s" s="70">
-        <v>4</v>
-      </c>
-      <c r="D5" s="71">
-        <v>4</v>
+        <v>64</v>
+      </c>
+      <c r="C5" t="s" s="67">
+        <v>5</v>
+      </c>
+      <c r="D5" s="68">
+        <v>10</v>
       </c>
       <c r="E5" s="46"/>
       <c r="F5" s="31"/>
@@ -6446,15 +6412,15 @@
       <c r="N5" s="31"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="69"/>
+      <c r="A6" s="70"/>
       <c r="B6" t="s" s="66">
-        <v>64</v>
-      </c>
-      <c r="C6" t="s" s="70">
-        <v>5</v>
-      </c>
-      <c r="D6" s="71">
-        <v>10</v>
+        <v>65</v>
+      </c>
+      <c r="C6" t="s" s="67">
+        <v>6</v>
+      </c>
+      <c r="D6" s="68">
+        <v>11</v>
       </c>
       <c r="E6" s="46"/>
       <c r="F6" s="31"/>
@@ -6468,15 +6434,15 @@
       <c r="N6" s="31"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="72"/>
+      <c r="A7" s="70"/>
       <c r="B7" t="s" s="66">
         <v>65</v>
       </c>
-      <c r="C7" t="s" s="70">
+      <c r="C7" t="s" s="67">
         <v>6</v>
       </c>
-      <c r="D7" s="71">
-        <v>11</v>
+      <c r="D7" s="68">
+        <v>12</v>
       </c>
       <c r="E7" s="46"/>
       <c r="F7" s="31"/>
@@ -6490,15 +6456,15 @@
       <c r="N7" s="31"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="72"/>
+      <c r="A8" s="70"/>
       <c r="B8" t="s" s="66">
-        <v>65</v>
-      </c>
-      <c r="C8" t="s" s="70">
-        <v>6</v>
-      </c>
-      <c r="D8" s="71">
-        <v>12</v>
+        <v>66</v>
+      </c>
+      <c r="C8" t="s" s="67">
+        <v>7</v>
+      </c>
+      <c r="D8" s="68">
+        <v>7</v>
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="31"/>
@@ -6512,15 +6478,15 @@
       <c r="N8" s="31"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="72"/>
+      <c r="A9" s="71"/>
       <c r="B9" t="s" s="66">
-        <v>66</v>
-      </c>
-      <c r="C9" t="s" s="70">
-        <v>7</v>
-      </c>
-      <c r="D9" s="71">
-        <v>7</v>
+        <v>67</v>
+      </c>
+      <c r="C9" t="s" s="67">
+        <v>8</v>
+      </c>
+      <c r="D9" s="68">
+        <v>4</v>
       </c>
       <c r="E9" s="46"/>
       <c r="F9" s="31"/>
@@ -6534,15 +6500,15 @@
       <c r="N9" s="31"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="73"/>
+      <c r="A10" s="71"/>
       <c r="B10" t="s" s="66">
-        <v>67</v>
-      </c>
-      <c r="C10" t="s" s="70">
-        <v>8</v>
-      </c>
-      <c r="D10" s="71">
-        <v>4</v>
+        <v>68</v>
+      </c>
+      <c r="C10" t="s" s="67">
+        <v>9</v>
+      </c>
+      <c r="D10" s="68">
+        <v>6</v>
       </c>
       <c r="E10" s="46"/>
       <c r="F10" s="31"/>
@@ -6556,15 +6522,15 @@
       <c r="N10" s="31"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="73"/>
+      <c r="A11" s="71"/>
       <c r="B11" t="s" s="66">
-        <v>68</v>
-      </c>
-      <c r="C11" t="s" s="70">
-        <v>9</v>
-      </c>
-      <c r="D11" s="71">
-        <v>6</v>
+        <v>69</v>
+      </c>
+      <c r="C11" t="s" s="67">
+        <v>10</v>
+      </c>
+      <c r="D11" s="68">
+        <v>3</v>
       </c>
       <c r="E11" s="46"/>
       <c r="F11" s="31"/>
@@ -6578,15 +6544,15 @@
       <c r="N11" s="31"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="73"/>
+      <c r="A12" s="71"/>
       <c r="B12" t="s" s="66">
-        <v>69</v>
-      </c>
-      <c r="C12" t="s" s="70">
-        <v>10</v>
-      </c>
-      <c r="D12" s="71">
-        <v>3</v>
+        <v>70</v>
+      </c>
+      <c r="C12" t="s" s="67">
+        <v>11</v>
+      </c>
+      <c r="D12" s="68">
+        <v>1</v>
       </c>
       <c r="E12" s="46"/>
       <c r="F12" s="31"/>
@@ -6600,15 +6566,15 @@
       <c r="N12" s="31"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="73"/>
+      <c r="A13" s="71"/>
       <c r="B13" t="s" s="66">
-        <v>70</v>
-      </c>
-      <c r="C13" t="s" s="70">
-        <v>11</v>
-      </c>
-      <c r="D13" s="71">
-        <v>1</v>
+        <v>71</v>
+      </c>
+      <c r="C13" t="s" s="67">
+        <v>12</v>
+      </c>
+      <c r="D13" s="68">
+        <v>6</v>
       </c>
       <c r="E13" s="46"/>
       <c r="F13" s="31"/>
@@ -6622,15 +6588,15 @@
       <c r="N13" s="31"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="73"/>
+      <c r="A14" s="71"/>
       <c r="B14" t="s" s="66">
-        <v>71</v>
-      </c>
-      <c r="C14" t="s" s="70">
-        <v>12</v>
-      </c>
-      <c r="D14" s="71">
-        <v>6</v>
+        <v>72</v>
+      </c>
+      <c r="C14" t="s" s="67">
+        <v>13</v>
+      </c>
+      <c r="D14" s="68">
+        <v>8</v>
       </c>
       <c r="E14" s="46"/>
       <c r="F14" s="31"/>
@@ -6644,15 +6610,15 @@
       <c r="N14" s="31"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="73"/>
+      <c r="A15" s="71"/>
       <c r="B15" t="s" s="66">
-        <v>72</v>
-      </c>
-      <c r="C15" t="s" s="70">
-        <v>13</v>
-      </c>
-      <c r="D15" s="71">
-        <v>8</v>
+        <v>73</v>
+      </c>
+      <c r="C15" t="s" s="67">
+        <v>14</v>
+      </c>
+      <c r="D15" s="68">
+        <v>9</v>
       </c>
       <c r="E15" s="46"/>
       <c r="F15" s="31"/>
@@ -6666,15 +6632,15 @@
       <c r="N15" s="31"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="73"/>
+      <c r="A16" s="71"/>
       <c r="B16" t="s" s="66">
-        <v>73</v>
-      </c>
-      <c r="C16" t="s" s="70">
-        <v>14</v>
-      </c>
-      <c r="D16" s="71">
-        <v>9</v>
+        <v>74</v>
+      </c>
+      <c r="C16" t="s" s="67">
+        <v>15</v>
+      </c>
+      <c r="D16" s="68">
+        <v>5</v>
       </c>
       <c r="E16" s="46"/>
       <c r="F16" s="31"/>
@@ -6688,15 +6654,15 @@
       <c r="N16" s="31"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="73"/>
+      <c r="A17" s="71"/>
       <c r="B17" t="s" s="66">
-        <v>74</v>
-      </c>
-      <c r="C17" t="s" s="70">
-        <v>15</v>
-      </c>
-      <c r="D17" s="71">
-        <v>5</v>
+        <v>75</v>
+      </c>
+      <c r="C17" t="s" s="67">
+        <v>16</v>
+      </c>
+      <c r="D17" s="68">
+        <v>4</v>
       </c>
       <c r="E17" s="46"/>
       <c r="F17" s="31"/>
@@ -6710,15 +6676,15 @@
       <c r="N17" s="31"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="73"/>
+      <c r="A18" s="71"/>
       <c r="B18" t="s" s="66">
-        <v>75</v>
-      </c>
-      <c r="C18" t="s" s="70">
-        <v>16</v>
-      </c>
-      <c r="D18" s="71">
-        <v>4</v>
+        <v>76</v>
+      </c>
+      <c r="C18" t="s" s="67">
+        <v>17</v>
+      </c>
+      <c r="D18" s="68">
+        <v>2</v>
       </c>
       <c r="E18" s="46"/>
       <c r="F18" s="31"/>
@@ -6732,15 +6698,15 @@
       <c r="N18" s="31"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="73"/>
+      <c r="A19" s="71"/>
       <c r="B19" t="s" s="66">
-        <v>76</v>
-      </c>
-      <c r="C19" t="s" s="70">
-        <v>17</v>
-      </c>
-      <c r="D19" s="71">
-        <v>2</v>
+        <v>77</v>
+      </c>
+      <c r="C19" t="s" s="67">
+        <v>18</v>
+      </c>
+      <c r="D19" s="68">
+        <v>5</v>
       </c>
       <c r="E19" s="46"/>
       <c r="F19" s="31"/>
@@ -6754,15 +6720,15 @@
       <c r="N19" s="31"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="73"/>
+      <c r="A20" s="71"/>
       <c r="B20" t="s" s="66">
-        <v>77</v>
-      </c>
-      <c r="C20" t="s" s="70">
-        <v>18</v>
-      </c>
-      <c r="D20" s="71">
-        <v>5</v>
+        <v>78</v>
+      </c>
+      <c r="C20" t="s" s="67">
+        <v>19</v>
+      </c>
+      <c r="D20" s="68">
+        <v>7</v>
       </c>
       <c r="E20" s="46"/>
       <c r="F20" s="31"/>
@@ -6776,15 +6742,15 @@
       <c r="N20" s="31"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="73"/>
+      <c r="A21" s="71"/>
       <c r="B21" t="s" s="66">
-        <v>78</v>
-      </c>
-      <c r="C21" t="s" s="70">
-        <v>19</v>
-      </c>
-      <c r="D21" s="71">
-        <v>7</v>
+        <v>79</v>
+      </c>
+      <c r="C21" t="s" s="67">
+        <v>20</v>
+      </c>
+      <c r="D21" s="68">
+        <v>15</v>
       </c>
       <c r="E21" s="46"/>
       <c r="F21" s="31"/>
@@ -6798,15 +6764,15 @@
       <c r="N21" s="31"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="73"/>
+      <c r="A22" s="71"/>
       <c r="B22" t="s" s="66">
-        <v>79</v>
-      </c>
-      <c r="C22" t="s" s="70">
-        <v>20</v>
-      </c>
-      <c r="D22" s="71">
-        <v>15</v>
+        <v>80</v>
+      </c>
+      <c r="C22" t="s" s="67">
+        <v>21</v>
+      </c>
+      <c r="D22" s="68">
+        <v>3</v>
       </c>
       <c r="E22" s="46"/>
       <c r="F22" s="31"/>
@@ -6820,15 +6786,15 @@
       <c r="N22" s="31"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="73"/>
+      <c r="A23" s="71"/>
       <c r="B23" t="s" s="66">
-        <v>80</v>
-      </c>
-      <c r="C23" t="s" s="70">
-        <v>21</v>
-      </c>
-      <c r="D23" s="71">
-        <v>3</v>
+        <v>81</v>
+      </c>
+      <c r="C23" t="s" s="67">
+        <v>22</v>
+      </c>
+      <c r="D23" s="68">
+        <v>7</v>
       </c>
       <c r="E23" s="46"/>
       <c r="F23" s="31"/>
@@ -6842,15 +6808,15 @@
       <c r="N23" s="31"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="73"/>
+      <c r="A24" s="71"/>
       <c r="B24" t="s" s="66">
-        <v>81</v>
-      </c>
-      <c r="C24" t="s" s="70">
-        <v>22</v>
-      </c>
-      <c r="D24" s="71">
-        <v>7</v>
+        <v>82</v>
+      </c>
+      <c r="C24" t="s" s="67">
+        <v>23</v>
+      </c>
+      <c r="D24" s="68">
+        <v>0</v>
       </c>
       <c r="E24" s="46"/>
       <c r="F24" s="31"/>
@@ -6864,15 +6830,15 @@
       <c r="N24" s="31"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="73"/>
+      <c r="A25" s="71"/>
       <c r="B25" t="s" s="66">
-        <v>82</v>
-      </c>
-      <c r="C25" t="s" s="70">
-        <v>23</v>
-      </c>
-      <c r="D25" s="71">
-        <v>0</v>
+        <v>83</v>
+      </c>
+      <c r="C25" t="s" s="67">
+        <v>24</v>
+      </c>
+      <c r="D25" s="68">
+        <v>3</v>
       </c>
       <c r="E25" s="46"/>
       <c r="F25" s="31"/>
@@ -6886,15 +6852,15 @@
       <c r="N25" s="31"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="73"/>
+      <c r="A26" s="71"/>
       <c r="B26" t="s" s="66">
-        <v>83</v>
-      </c>
-      <c r="C26" t="s" s="70">
-        <v>24</v>
-      </c>
-      <c r="D26" s="71">
-        <v>3</v>
+        <v>84</v>
+      </c>
+      <c r="C26" t="s" s="67">
+        <v>25</v>
+      </c>
+      <c r="D26" s="68">
+        <v>7</v>
       </c>
       <c r="E26" s="46"/>
       <c r="F26" s="31"/>
@@ -6908,15 +6874,15 @@
       <c r="N26" s="31"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="73"/>
+      <c r="A27" s="71"/>
       <c r="B27" t="s" s="66">
-        <v>84</v>
-      </c>
-      <c r="C27" t="s" s="70">
-        <v>25</v>
-      </c>
-      <c r="D27" s="71">
-        <v>7</v>
+        <v>85</v>
+      </c>
+      <c r="C27" t="s" s="67">
+        <v>26</v>
+      </c>
+      <c r="D27" s="68">
+        <v>3</v>
       </c>
       <c r="E27" s="46"/>
       <c r="F27" s="31"/>
@@ -6930,15 +6896,15 @@
       <c r="N27" s="31"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="73"/>
+      <c r="A28" s="71"/>
       <c r="B28" t="s" s="66">
-        <v>85</v>
-      </c>
-      <c r="C28" t="s" s="70">
-        <v>26</v>
-      </c>
-      <c r="D28" s="71">
-        <v>3</v>
+        <v>86</v>
+      </c>
+      <c r="C28" t="s" s="67">
+        <v>27</v>
+      </c>
+      <c r="D28" s="68">
+        <v>2</v>
       </c>
       <c r="E28" s="46"/>
       <c r="F28" s="31"/>
@@ -6952,15 +6918,15 @@
       <c r="N28" s="31"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="73"/>
+      <c r="A29" s="71"/>
       <c r="B29" t="s" s="66">
-        <v>86</v>
-      </c>
-      <c r="C29" t="s" s="70">
-        <v>27</v>
-      </c>
-      <c r="D29" s="71">
-        <v>2</v>
+        <v>87</v>
+      </c>
+      <c r="C29" t="s" s="67">
+        <v>28</v>
+      </c>
+      <c r="D29" s="68">
+        <v>5</v>
       </c>
       <c r="E29" s="46"/>
       <c r="F29" s="31"/>
@@ -6974,15 +6940,15 @@
       <c r="N29" s="31"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="73"/>
+      <c r="A30" s="71"/>
       <c r="B30" t="s" s="66">
-        <v>87</v>
-      </c>
-      <c r="C30" t="s" s="70">
-        <v>28</v>
-      </c>
-      <c r="D30" s="71">
-        <v>5</v>
+        <v>88</v>
+      </c>
+      <c r="C30" t="s" s="67">
+        <v>29</v>
+      </c>
+      <c r="D30" s="68">
+        <v>7</v>
       </c>
       <c r="E30" s="46"/>
       <c r="F30" s="31"/>
@@ -6996,15 +6962,15 @@
       <c r="N30" s="31"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="73"/>
+      <c r="A31" s="71"/>
       <c r="B31" t="s" s="66">
-        <v>88</v>
-      </c>
-      <c r="C31" t="s" s="70">
-        <v>29</v>
-      </c>
-      <c r="D31" s="71">
-        <v>7</v>
+        <v>89</v>
+      </c>
+      <c r="C31" t="s" s="67">
+        <v>30</v>
+      </c>
+      <c r="D31" s="68">
+        <v>4</v>
       </c>
       <c r="E31" s="46"/>
       <c r="F31" s="31"/>
@@ -7018,14 +6984,14 @@
       <c r="N31" s="31"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="73"/>
+      <c r="A32" s="71"/>
       <c r="B32" t="s" s="66">
-        <v>89</v>
-      </c>
-      <c r="C32" t="s" s="70">
-        <v>30</v>
-      </c>
-      <c r="D32" s="71">
+        <v>90</v>
+      </c>
+      <c r="C32" t="s" s="67">
+        <v>31</v>
+      </c>
+      <c r="D32" s="68">
         <v>4</v>
       </c>
       <c r="E32" s="46"/>
@@ -7040,15 +7006,15 @@
       <c r="N32" s="31"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="73"/>
+      <c r="A33" s="71"/>
       <c r="B33" t="s" s="66">
-        <v>90</v>
-      </c>
-      <c r="C33" t="s" s="70">
-        <v>31</v>
-      </c>
-      <c r="D33" s="71">
-        <v>4</v>
+        <v>124</v>
+      </c>
+      <c r="C33" t="s" s="67">
+        <v>32</v>
+      </c>
+      <c r="D33" s="68">
+        <v>2</v>
       </c>
       <c r="E33" s="46"/>
       <c r="F33" s="31"/>
@@ -7062,15 +7028,15 @@
       <c r="N33" s="31"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="73"/>
+      <c r="A34" s="71"/>
       <c r="B34" t="s" s="66">
-        <v>125</v>
-      </c>
-      <c r="C34" t="s" s="70">
-        <v>32</v>
-      </c>
-      <c r="D34" s="71">
-        <v>2</v>
+        <v>92</v>
+      </c>
+      <c r="C34" t="s" s="67">
+        <v>33</v>
+      </c>
+      <c r="D34" s="68">
+        <v>5</v>
       </c>
       <c r="E34" s="46"/>
       <c r="F34" s="31"/>
@@ -7084,15 +7050,15 @@
       <c r="N34" s="31"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="73"/>
+      <c r="A35" s="71"/>
       <c r="B35" t="s" s="66">
-        <v>92</v>
-      </c>
-      <c r="C35" t="s" s="70">
-        <v>33</v>
-      </c>
-      <c r="D35" s="71">
-        <v>5</v>
+        <v>93</v>
+      </c>
+      <c r="C35" t="s" s="67">
+        <v>34</v>
+      </c>
+      <c r="D35" s="68">
+        <v>7</v>
       </c>
       <c r="E35" s="46"/>
       <c r="F35" s="31"/>
@@ -7106,15 +7072,15 @@
       <c r="N35" s="31"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="73"/>
+      <c r="A36" s="71"/>
       <c r="B36" t="s" s="66">
-        <v>93</v>
-      </c>
-      <c r="C36" t="s" s="70">
-        <v>34</v>
-      </c>
-      <c r="D36" s="71">
-        <v>7</v>
+        <v>94</v>
+      </c>
+      <c r="C36" t="s" s="67">
+        <v>35</v>
+      </c>
+      <c r="D36" s="68">
+        <v>9</v>
       </c>
       <c r="E36" s="46"/>
       <c r="F36" s="31"/>
@@ -7128,15 +7094,15 @@
       <c r="N36" s="31"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="73"/>
+      <c r="A37" s="71"/>
       <c r="B37" t="s" s="66">
-        <v>94</v>
-      </c>
-      <c r="C37" t="s" s="70">
-        <v>35</v>
-      </c>
-      <c r="D37" s="71">
-        <v>9</v>
+        <v>95</v>
+      </c>
+      <c r="C37" t="s" s="67">
+        <v>36</v>
+      </c>
+      <c r="D37" s="68">
+        <v>4</v>
       </c>
       <c r="E37" s="46"/>
       <c r="F37" s="31"/>
@@ -7150,15 +7116,15 @@
       <c r="N37" s="31"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="73"/>
+      <c r="A38" s="71"/>
       <c r="B38" t="s" s="66">
-        <v>95</v>
-      </c>
-      <c r="C38" t="s" s="70">
-        <v>36</v>
-      </c>
-      <c r="D38" s="71">
-        <v>4</v>
+        <v>96</v>
+      </c>
+      <c r="C38" t="s" s="67">
+        <v>37</v>
+      </c>
+      <c r="D38" s="68">
+        <v>2</v>
       </c>
       <c r="E38" s="46"/>
       <c r="F38" s="31"/>
@@ -7172,15 +7138,15 @@
       <c r="N38" s="31"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="73"/>
+      <c r="A39" s="71"/>
       <c r="B39" t="s" s="66">
-        <v>96</v>
-      </c>
-      <c r="C39" t="s" s="70">
-        <v>37</v>
-      </c>
-      <c r="D39" s="71">
-        <v>2</v>
+        <v>97</v>
+      </c>
+      <c r="C39" t="s" s="67">
+        <v>38</v>
+      </c>
+      <c r="D39" s="68">
+        <v>6</v>
       </c>
       <c r="E39" s="46"/>
       <c r="F39" s="31"/>
@@ -7194,15 +7160,15 @@
       <c r="N39" s="31"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="73"/>
+      <c r="A40" s="71"/>
       <c r="B40" t="s" s="66">
-        <v>97</v>
-      </c>
-      <c r="C40" t="s" s="70">
-        <v>38</v>
-      </c>
-      <c r="D40" s="71">
-        <v>6</v>
+        <v>98</v>
+      </c>
+      <c r="C40" t="s" s="67">
+        <v>39</v>
+      </c>
+      <c r="D40" s="68">
+        <v>3</v>
       </c>
       <c r="E40" s="46"/>
       <c r="F40" s="31"/>
@@ -7216,15 +7182,15 @@
       <c r="N40" s="31"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="73"/>
+      <c r="A41" s="71"/>
       <c r="B41" t="s" s="66">
-        <v>98</v>
-      </c>
-      <c r="C41" t="s" s="70">
-        <v>39</v>
-      </c>
-      <c r="D41" s="71">
-        <v>3</v>
+        <v>99</v>
+      </c>
+      <c r="C41" t="s" s="67">
+        <v>40</v>
+      </c>
+      <c r="D41" s="68">
+        <v>2</v>
       </c>
       <c r="E41" s="46"/>
       <c r="F41" s="31"/>
@@ -7238,15 +7204,15 @@
       <c r="N41" s="31"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="73"/>
+      <c r="A42" s="71"/>
       <c r="B42" t="s" s="66">
-        <v>99</v>
-      </c>
-      <c r="C42" t="s" s="70">
-        <v>40</v>
-      </c>
-      <c r="D42" s="71">
-        <v>2</v>
+        <v>100</v>
+      </c>
+      <c r="C42" t="s" s="67">
+        <v>41</v>
+      </c>
+      <c r="D42" s="68">
+        <v>6</v>
       </c>
       <c r="E42" s="46"/>
       <c r="F42" s="31"/>
@@ -7260,15 +7226,15 @@
       <c r="N42" s="31"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="73"/>
+      <c r="A43" s="71"/>
       <c r="B43" t="s" s="66">
-        <v>100</v>
-      </c>
-      <c r="C43" t="s" s="70">
-        <v>41</v>
-      </c>
-      <c r="D43" s="71">
-        <v>6</v>
+        <v>101</v>
+      </c>
+      <c r="C43" t="s" s="67">
+        <v>42</v>
+      </c>
+      <c r="D43" s="68">
+        <v>5</v>
       </c>
       <c r="E43" s="46"/>
       <c r="F43" s="31"/>
@@ -7282,15 +7248,15 @@
       <c r="N43" s="31"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="73"/>
+      <c r="A44" s="71"/>
       <c r="B44" t="s" s="66">
-        <v>101</v>
-      </c>
-      <c r="C44" t="s" s="70">
-        <v>42</v>
-      </c>
-      <c r="D44" s="71">
-        <v>5</v>
+        <v>102</v>
+      </c>
+      <c r="C44" t="s" s="67">
+        <v>43</v>
+      </c>
+      <c r="D44" s="68">
+        <v>3</v>
       </c>
       <c r="E44" s="46"/>
       <c r="F44" s="31"/>
@@ -7304,15 +7270,15 @@
       <c r="N44" s="31"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="73"/>
+      <c r="A45" s="71"/>
       <c r="B45" t="s" s="66">
-        <v>102</v>
-      </c>
-      <c r="C45" t="s" s="70">
-        <v>43</v>
-      </c>
-      <c r="D45" s="71">
-        <v>3</v>
+        <v>103</v>
+      </c>
+      <c r="C45" t="s" s="67">
+        <v>44</v>
+      </c>
+      <c r="D45" s="68">
+        <v>5</v>
       </c>
       <c r="E45" s="46"/>
       <c r="F45" s="31"/>
@@ -7326,15 +7292,15 @@
       <c r="N45" s="31"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="73"/>
+      <c r="A46" s="71"/>
       <c r="B46" t="s" s="66">
-        <v>103</v>
-      </c>
-      <c r="C46" t="s" s="70">
-        <v>44</v>
-      </c>
-      <c r="D46" s="71">
-        <v>5</v>
+        <v>104</v>
+      </c>
+      <c r="C46" t="s" s="67">
+        <v>45</v>
+      </c>
+      <c r="D46" s="68">
+        <v>36</v>
       </c>
       <c r="E46" s="46"/>
       <c r="F46" s="31"/>
@@ -7348,15 +7314,15 @@
       <c r="N46" s="31"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="73"/>
+      <c r="A47" s="71"/>
       <c r="B47" t="s" s="66">
-        <v>104</v>
-      </c>
-      <c r="C47" t="s" s="70">
-        <v>45</v>
-      </c>
-      <c r="D47" s="71">
-        <v>36</v>
+        <v>105</v>
+      </c>
+      <c r="C47" t="s" s="67">
+        <v>46</v>
+      </c>
+      <c r="D47" s="68">
+        <v>7</v>
       </c>
       <c r="E47" s="46"/>
       <c r="F47" s="31"/>
@@ -7370,15 +7336,15 @@
       <c r="N47" s="31"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="73"/>
+      <c r="A48" s="71"/>
       <c r="B48" t="s" s="66">
-        <v>105</v>
-      </c>
-      <c r="C48" t="s" s="70">
-        <v>46</v>
-      </c>
-      <c r="D48" s="71">
-        <v>7</v>
+        <v>106</v>
+      </c>
+      <c r="C48" t="s" s="67">
+        <v>47</v>
+      </c>
+      <c r="D48" s="68">
+        <v>1</v>
       </c>
       <c r="E48" s="46"/>
       <c r="F48" s="31"/>
@@ -7392,15 +7358,15 @@
       <c r="N48" s="31"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="73"/>
+      <c r="A49" s="71"/>
       <c r="B49" t="s" s="66">
-        <v>106</v>
-      </c>
-      <c r="C49" t="s" s="70">
-        <v>47</v>
-      </c>
-      <c r="D49" s="71">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="C49" t="s" s="67">
+        <v>48</v>
+      </c>
+      <c r="D49" s="68">
+        <v>4</v>
       </c>
       <c r="E49" s="46"/>
       <c r="F49" s="31"/>
@@ -7414,15 +7380,15 @@
       <c r="N49" s="31"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="73"/>
+      <c r="A50" s="71"/>
       <c r="B50" t="s" s="66">
-        <v>107</v>
-      </c>
-      <c r="C50" t="s" s="70">
-        <v>48</v>
-      </c>
-      <c r="D50" s="71">
-        <v>4</v>
+        <v>108</v>
+      </c>
+      <c r="C50" t="s" s="67">
+        <v>49</v>
+      </c>
+      <c r="D50" s="68">
+        <v>57</v>
       </c>
       <c r="E50" s="46"/>
       <c r="F50" s="31"/>
@@ -7436,15 +7402,15 @@
       <c r="N50" s="31"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="73"/>
+      <c r="A51" s="71"/>
       <c r="B51" t="s" s="66">
-        <v>108</v>
-      </c>
-      <c r="C51" t="s" s="70">
-        <v>49</v>
-      </c>
-      <c r="D51" s="71">
-        <v>57</v>
+        <v>109</v>
+      </c>
+      <c r="C51" t="s" s="67">
+        <v>50</v>
+      </c>
+      <c r="D51" s="68">
+        <v>3</v>
       </c>
       <c r="E51" s="46"/>
       <c r="F51" s="31"/>
@@ -7458,15 +7424,15 @@
       <c r="N51" s="31"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="73"/>
+      <c r="A52" s="71"/>
       <c r="B52" t="s" s="66">
-        <v>109</v>
-      </c>
-      <c r="C52" t="s" s="70">
-        <v>50</v>
-      </c>
-      <c r="D52" s="71">
-        <v>3</v>
+        <v>110</v>
+      </c>
+      <c r="C52" t="s" s="67">
+        <v>51</v>
+      </c>
+      <c r="D52" s="68">
+        <v>1</v>
       </c>
       <c r="E52" s="46"/>
       <c r="F52" s="31"/>
@@ -7480,15 +7446,15 @@
       <c r="N52" s="31"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="73"/>
+      <c r="A53" s="71"/>
       <c r="B53" t="s" s="66">
-        <v>110</v>
-      </c>
-      <c r="C53" t="s" s="70">
-        <v>51</v>
-      </c>
-      <c r="D53" s="71">
-        <v>1</v>
+        <v>111</v>
+      </c>
+      <c r="C53" t="s" s="67">
+        <v>52</v>
+      </c>
+      <c r="D53" s="68">
+        <v>7</v>
       </c>
       <c r="E53" s="46"/>
       <c r="F53" s="31"/>
@@ -7502,15 +7468,15 @@
       <c r="N53" s="31"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="73"/>
+      <c r="A54" s="71"/>
       <c r="B54" t="s" s="66">
-        <v>111</v>
-      </c>
-      <c r="C54" t="s" s="70">
-        <v>52</v>
-      </c>
-      <c r="D54" s="71">
-        <v>7</v>
+        <v>112</v>
+      </c>
+      <c r="C54" t="s" s="67">
+        <v>53</v>
+      </c>
+      <c r="D54" s="68">
+        <v>4</v>
       </c>
       <c r="E54" s="46"/>
       <c r="F54" s="31"/>
@@ -7524,15 +7490,15 @@
       <c r="N54" s="31"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="73"/>
+      <c r="A55" s="71"/>
       <c r="B55" t="s" s="66">
-        <v>112</v>
-      </c>
-      <c r="C55" t="s" s="70">
-        <v>53</v>
-      </c>
-      <c r="D55" s="71">
-        <v>4</v>
+        <v>113</v>
+      </c>
+      <c r="C55" t="s" s="67">
+        <v>54</v>
+      </c>
+      <c r="D55" s="68">
+        <v>2</v>
       </c>
       <c r="E55" s="46"/>
       <c r="F55" s="31"/>
@@ -7546,15 +7512,15 @@
       <c r="N55" s="31"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="73"/>
+      <c r="A56" s="71"/>
       <c r="B56" t="s" s="66">
-        <v>113</v>
-      </c>
-      <c r="C56" t="s" s="70">
-        <v>54</v>
-      </c>
-      <c r="D56" s="71">
-        <v>2</v>
+        <v>114</v>
+      </c>
+      <c r="C56" t="s" s="67">
+        <v>55</v>
+      </c>
+      <c r="D56" s="68">
+        <v>6</v>
       </c>
       <c r="E56" s="46"/>
       <c r="F56" s="31"/>
@@ -7568,15 +7534,15 @@
       <c r="N56" s="31"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="73"/>
+      <c r="A57" s="71"/>
       <c r="B57" t="s" s="66">
-        <v>114</v>
-      </c>
-      <c r="C57" t="s" s="70">
-        <v>55</v>
-      </c>
-      <c r="D57" s="71">
-        <v>6</v>
+        <v>115</v>
+      </c>
+      <c r="C57" t="s" s="67">
+        <v>56</v>
+      </c>
+      <c r="D57" s="68">
+        <v>8</v>
       </c>
       <c r="E57" s="46"/>
       <c r="F57" s="31"/>
@@ -7590,15 +7556,15 @@
       <c r="N57" s="31"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="73"/>
+      <c r="A58" s="71"/>
       <c r="B58" t="s" s="66">
-        <v>115</v>
-      </c>
-      <c r="C58" t="s" s="70">
-        <v>56</v>
-      </c>
-      <c r="D58" s="71">
-        <v>8</v>
+        <v>116</v>
+      </c>
+      <c r="C58" t="s" s="67">
+        <v>57</v>
+      </c>
+      <c r="D58" s="68">
+        <v>2</v>
       </c>
       <c r="E58" s="46"/>
       <c r="F58" s="31"/>
@@ -7612,14 +7578,14 @@
       <c r="N58" s="31"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="73"/>
+      <c r="A59" s="71"/>
       <c r="B59" t="s" s="66">
-        <v>116</v>
-      </c>
-      <c r="C59" t="s" s="70">
-        <v>57</v>
-      </c>
-      <c r="D59" s="71">
+        <v>117</v>
+      </c>
+      <c r="C59" t="s" s="67">
+        <v>58</v>
+      </c>
+      <c r="D59" s="68">
         <v>2</v>
       </c>
       <c r="E59" s="46"/>
@@ -7634,15 +7600,15 @@
       <c r="N59" s="31"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="73"/>
+      <c r="A60" s="71"/>
       <c r="B60" t="s" s="66">
-        <v>117</v>
-      </c>
-      <c r="C60" t="s" s="70">
-        <v>58</v>
-      </c>
-      <c r="D60" s="71">
-        <v>2</v>
+        <v>118</v>
+      </c>
+      <c r="C60" t="s" s="67">
+        <v>59</v>
+      </c>
+      <c r="D60" s="68">
+        <v>6</v>
       </c>
       <c r="E60" s="46"/>
       <c r="F60" s="31"/>
@@ -7656,15 +7622,15 @@
       <c r="N60" s="31"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="73"/>
+      <c r="A61" s="71"/>
       <c r="B61" t="s" s="66">
-        <v>118</v>
-      </c>
-      <c r="C61" t="s" s="70">
-        <v>59</v>
-      </c>
-      <c r="D61" s="71">
-        <v>6</v>
+        <v>119</v>
+      </c>
+      <c r="C61" t="s" s="67">
+        <v>60</v>
+      </c>
+      <c r="D61" s="68">
+        <v>1</v>
       </c>
       <c r="E61" s="46"/>
       <c r="F61" s="31"/>
@@ -7678,16 +7644,10 @@
       <c r="N61" s="31"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="73"/>
-      <c r="B62" t="s" s="66">
-        <v>119</v>
-      </c>
-      <c r="C62" t="s" s="70">
-        <v>60</v>
-      </c>
-      <c r="D62" s="71">
-        <v>1</v>
-      </c>
+      <c r="A62" s="71"/>
+      <c r="B62" s="72"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="68"/>
       <c r="E62" s="46"/>
       <c r="F62" s="31"/>
       <c r="G62" s="31"/>
@@ -7700,10 +7660,10 @@
       <c r="N62" s="31"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="73"/>
-      <c r="B63" s="67"/>
+      <c r="A63" s="71"/>
+      <c r="B63" s="46"/>
       <c r="C63" s="31"/>
-      <c r="D63" s="71"/>
+      <c r="D63" s="68"/>
       <c r="E63" s="46"/>
       <c r="F63" s="31"/>
       <c r="G63" s="31"/>
@@ -7716,10 +7676,10 @@
       <c r="N63" s="31"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="73"/>
+      <c r="A64" s="71"/>
       <c r="B64" s="46"/>
       <c r="C64" s="31"/>
-      <c r="D64" s="71"/>
+      <c r="D64" s="68"/>
       <c r="E64" s="46"/>
       <c r="F64" s="31"/>
       <c r="G64" s="31"/>
@@ -7732,10 +7692,10 @@
       <c r="N64" s="31"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="73"/>
+      <c r="A65" s="71"/>
       <c r="B65" s="46"/>
       <c r="C65" s="31"/>
-      <c r="D65" s="71"/>
+      <c r="D65" s="68"/>
       <c r="E65" s="46"/>
       <c r="F65" s="31"/>
       <c r="G65" s="31"/>
@@ -7748,10 +7708,10 @@
       <c r="N65" s="31"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="73"/>
+      <c r="A66" s="71"/>
       <c r="B66" s="46"/>
       <c r="C66" s="31"/>
-      <c r="D66" s="71"/>
+      <c r="D66" s="68"/>
       <c r="E66" s="46"/>
       <c r="F66" s="31"/>
       <c r="G66" s="31"/>
@@ -7764,10 +7724,10 @@
       <c r="N66" s="31"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="73"/>
+      <c r="A67" s="71"/>
       <c r="B67" s="46"/>
       <c r="C67" s="31"/>
-      <c r="D67" s="71"/>
+      <c r="D67" s="68"/>
       <c r="E67" s="46"/>
       <c r="F67" s="31"/>
       <c r="G67" s="31"/>
@@ -7780,10 +7740,10 @@
       <c r="N67" s="31"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="73"/>
+      <c r="A68" s="71"/>
       <c r="B68" s="46"/>
       <c r="C68" s="31"/>
-      <c r="D68" s="71"/>
+      <c r="D68" s="68"/>
       <c r="E68" s="46"/>
       <c r="F68" s="31"/>
       <c r="G68" s="31"/>
@@ -7796,10 +7756,10 @@
       <c r="N68" s="31"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="73"/>
+      <c r="A69" s="71"/>
       <c r="B69" s="46"/>
       <c r="C69" s="31"/>
-      <c r="D69" s="71"/>
+      <c r="D69" s="68"/>
       <c r="E69" s="46"/>
       <c r="F69" s="31"/>
       <c r="G69" s="31"/>
@@ -7812,10 +7772,10 @@
       <c r="N69" s="31"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="73"/>
+      <c r="A70" s="71"/>
       <c r="B70" s="46"/>
       <c r="C70" s="31"/>
-      <c r="D70" s="71"/>
+      <c r="D70" s="68"/>
       <c r="E70" s="46"/>
       <c r="F70" s="31"/>
       <c r="G70" s="31"/>
@@ -7828,10 +7788,10 @@
       <c r="N70" s="31"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="73"/>
+      <c r="A71" s="71"/>
       <c r="B71" s="46"/>
       <c r="C71" s="31"/>
-      <c r="D71" s="71"/>
+      <c r="D71" s="68"/>
       <c r="E71" s="46"/>
       <c r="F71" s="31"/>
       <c r="G71" s="31"/>
@@ -7844,10 +7804,10 @@
       <c r="N71" s="31"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="73"/>
+      <c r="A72" s="71"/>
       <c r="B72" s="46"/>
       <c r="C72" s="31"/>
-      <c r="D72" s="71"/>
+      <c r="D72" s="68"/>
       <c r="E72" s="46"/>
       <c r="F72" s="31"/>
       <c r="G72" s="31"/>
@@ -7860,10 +7820,10 @@
       <c r="N72" s="31"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="73"/>
+      <c r="A73" s="71"/>
       <c r="B73" s="46"/>
       <c r="C73" s="31"/>
-      <c r="D73" s="71"/>
+      <c r="D73" s="68"/>
       <c r="E73" s="46"/>
       <c r="F73" s="31"/>
       <c r="G73" s="31"/>
@@ -7876,10 +7836,10 @@
       <c r="N73" s="31"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="73"/>
+      <c r="A74" s="71"/>
       <c r="B74" s="46"/>
       <c r="C74" s="31"/>
-      <c r="D74" s="71"/>
+      <c r="D74" s="68"/>
       <c r="E74" s="46"/>
       <c r="F74" s="31"/>
       <c r="G74" s="31"/>
@@ -7892,10 +7852,10 @@
       <c r="N74" s="31"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="73"/>
+      <c r="A75" s="71"/>
       <c r="B75" s="46"/>
       <c r="C75" s="31"/>
-      <c r="D75" s="71"/>
+      <c r="D75" s="68"/>
       <c r="E75" s="46"/>
       <c r="F75" s="31"/>
       <c r="G75" s="31"/>
@@ -7908,10 +7868,10 @@
       <c r="N75" s="31"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="73"/>
+      <c r="A76" s="71"/>
       <c r="B76" s="46"/>
       <c r="C76" s="31"/>
-      <c r="D76" s="71"/>
+      <c r="D76" s="68"/>
       <c r="E76" s="46"/>
       <c r="F76" s="31"/>
       <c r="G76" s="31"/>
@@ -7924,10 +7884,10 @@
       <c r="N76" s="31"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="73"/>
+      <c r="A77" s="71"/>
       <c r="B77" s="46"/>
       <c r="C77" s="31"/>
-      <c r="D77" s="71"/>
+      <c r="D77" s="68"/>
       <c r="E77" s="46"/>
       <c r="F77" s="31"/>
       <c r="G77" s="31"/>
@@ -7940,10 +7900,10 @@
       <c r="N77" s="31"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="73"/>
+      <c r="A78" s="71"/>
       <c r="B78" s="46"/>
       <c r="C78" s="31"/>
-      <c r="D78" s="71"/>
+      <c r="D78" s="68"/>
       <c r="E78" s="46"/>
       <c r="F78" s="31"/>
       <c r="G78" s="31"/>
@@ -7956,10 +7916,10 @@
       <c r="N78" s="31"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="73"/>
+      <c r="A79" s="71"/>
       <c r="B79" s="46"/>
       <c r="C79" s="31"/>
-      <c r="D79" s="71"/>
+      <c r="D79" s="68"/>
       <c r="E79" s="46"/>
       <c r="F79" s="31"/>
       <c r="G79" s="31"/>
@@ -7972,10 +7932,10 @@
       <c r="N79" s="31"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="73"/>
+      <c r="A80" s="71"/>
       <c r="B80" s="46"/>
       <c r="C80" s="31"/>
-      <c r="D80" s="71"/>
+      <c r="D80" s="68"/>
       <c r="E80" s="46"/>
       <c r="F80" s="31"/>
       <c r="G80" s="31"/>
@@ -7988,10 +7948,10 @@
       <c r="N80" s="31"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="73"/>
+      <c r="A81" s="71"/>
       <c r="B81" s="46"/>
       <c r="C81" s="31"/>
-      <c r="D81" s="71"/>
+      <c r="D81" s="68"/>
       <c r="E81" s="46"/>
       <c r="F81" s="31"/>
       <c r="G81" s="31"/>
@@ -8004,10 +7964,10 @@
       <c r="N81" s="31"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="73"/>
+      <c r="A82" s="71"/>
       <c r="B82" s="46"/>
       <c r="C82" s="31"/>
-      <c r="D82" s="71"/>
+      <c r="D82" s="68"/>
       <c r="E82" s="46"/>
       <c r="F82" s="31"/>
       <c r="G82" s="31"/>
@@ -8020,10 +7980,10 @@
       <c r="N82" s="31"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="73"/>
+      <c r="A83" s="71"/>
       <c r="B83" s="46"/>
       <c r="C83" s="31"/>
-      <c r="D83" s="71"/>
+      <c r="D83" s="68"/>
       <c r="E83" s="46"/>
       <c r="F83" s="31"/>
       <c r="G83" s="31"/>
@@ -8036,10 +7996,10 @@
       <c r="N83" s="31"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="73"/>
+      <c r="A84" s="71"/>
       <c r="B84" s="46"/>
       <c r="C84" s="31"/>
-      <c r="D84" s="71"/>
+      <c r="D84" s="68"/>
       <c r="E84" s="46"/>
       <c r="F84" s="31"/>
       <c r="G84" s="31"/>
@@ -8052,10 +8012,10 @@
       <c r="N84" s="31"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="73"/>
+      <c r="A85" s="71"/>
       <c r="B85" s="46"/>
       <c r="C85" s="31"/>
-      <c r="D85" s="71"/>
+      <c r="D85" s="68"/>
       <c r="E85" s="46"/>
       <c r="F85" s="31"/>
       <c r="G85" s="31"/>
@@ -8068,10 +8028,10 @@
       <c r="N85" s="31"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="73"/>
+      <c r="A86" s="71"/>
       <c r="B86" s="46"/>
       <c r="C86" s="31"/>
-      <c r="D86" s="71"/>
+      <c r="D86" s="68"/>
       <c r="E86" s="46"/>
       <c r="F86" s="31"/>
       <c r="G86" s="31"/>
@@ -8084,10 +8044,10 @@
       <c r="N86" s="31"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="73"/>
+      <c r="A87" s="71"/>
       <c r="B87" s="46"/>
       <c r="C87" s="31"/>
-      <c r="D87" s="71"/>
+      <c r="D87" s="68"/>
       <c r="E87" s="46"/>
       <c r="F87" s="31"/>
       <c r="G87" s="31"/>
@@ -8100,10 +8060,10 @@
       <c r="N87" s="31"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="73"/>
+      <c r="A88" s="71"/>
       <c r="B88" s="46"/>
       <c r="C88" s="31"/>
-      <c r="D88" s="71"/>
+      <c r="D88" s="68"/>
       <c r="E88" s="46"/>
       <c r="F88" s="31"/>
       <c r="G88" s="31"/>
@@ -8116,10 +8076,10 @@
       <c r="N88" s="31"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="73"/>
+      <c r="A89" s="71"/>
       <c r="B89" s="46"/>
       <c r="C89" s="31"/>
-      <c r="D89" s="71"/>
+      <c r="D89" s="68"/>
       <c r="E89" s="46"/>
       <c r="F89" s="31"/>
       <c r="G89" s="31"/>
@@ -8132,10 +8092,10 @@
       <c r="N89" s="31"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="73"/>
+      <c r="A90" s="71"/>
       <c r="B90" s="46"/>
       <c r="C90" s="31"/>
-      <c r="D90" s="71"/>
+      <c r="D90" s="68"/>
       <c r="E90" s="46"/>
       <c r="F90" s="31"/>
       <c r="G90" s="31"/>
@@ -8148,10 +8108,10 @@
       <c r="N90" s="31"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="73"/>
+      <c r="A91" s="71"/>
       <c r="B91" s="46"/>
       <c r="C91" s="31"/>
-      <c r="D91" s="71"/>
+      <c r="D91" s="68"/>
       <c r="E91" s="46"/>
       <c r="F91" s="31"/>
       <c r="G91" s="31"/>
@@ -8164,10 +8124,10 @@
       <c r="N91" s="31"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="73"/>
+      <c r="A92" s="71"/>
       <c r="B92" s="46"/>
       <c r="C92" s="31"/>
-      <c r="D92" s="71"/>
+      <c r="D92" s="68"/>
       <c r="E92" s="46"/>
       <c r="F92" s="31"/>
       <c r="G92" s="31"/>
@@ -8180,10 +8140,10 @@
       <c r="N92" s="31"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="73"/>
+      <c r="A93" s="71"/>
       <c r="B93" s="46"/>
       <c r="C93" s="31"/>
-      <c r="D93" s="71"/>
+      <c r="D93" s="68"/>
       <c r="E93" s="46"/>
       <c r="F93" s="31"/>
       <c r="G93" s="31"/>
@@ -8196,10 +8156,10 @@
       <c r="N93" s="31"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="73"/>
+      <c r="A94" s="71"/>
       <c r="B94" s="46"/>
       <c r="C94" s="31"/>
-      <c r="D94" s="71"/>
+      <c r="D94" s="68"/>
       <c r="E94" s="46"/>
       <c r="F94" s="31"/>
       <c r="G94" s="31"/>
@@ -8212,10 +8172,10 @@
       <c r="N94" s="31"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="73"/>
+      <c r="A95" s="71"/>
       <c r="B95" s="46"/>
       <c r="C95" s="31"/>
-      <c r="D95" s="71"/>
+      <c r="D95" s="68"/>
       <c r="E95" s="46"/>
       <c r="F95" s="31"/>
       <c r="G95" s="31"/>
@@ -8228,10 +8188,10 @@
       <c r="N95" s="31"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="73"/>
+      <c r="A96" s="71"/>
       <c r="B96" s="46"/>
       <c r="C96" s="31"/>
-      <c r="D96" s="71"/>
+      <c r="D96" s="68"/>
       <c r="E96" s="46"/>
       <c r="F96" s="31"/>
       <c r="G96" s="31"/>
@@ -8244,10 +8204,10 @@
       <c r="N96" s="31"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="73"/>
+      <c r="A97" s="71"/>
       <c r="B97" s="46"/>
       <c r="C97" s="31"/>
-      <c r="D97" s="71"/>
+      <c r="D97" s="68"/>
       <c r="E97" s="46"/>
       <c r="F97" s="31"/>
       <c r="G97" s="31"/>
@@ -8260,10 +8220,10 @@
       <c r="N97" s="31"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="73"/>
+      <c r="A98" s="71"/>
       <c r="B98" s="46"/>
       <c r="C98" s="31"/>
-      <c r="D98" s="71"/>
+      <c r="D98" s="68"/>
       <c r="E98" s="46"/>
       <c r="F98" s="31"/>
       <c r="G98" s="31"/>
@@ -8276,10 +8236,10 @@
       <c r="N98" s="31"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="73"/>
+      <c r="A99" s="71"/>
       <c r="B99" s="46"/>
       <c r="C99" s="31"/>
-      <c r="D99" s="71"/>
+      <c r="D99" s="68"/>
       <c r="E99" s="46"/>
       <c r="F99" s="31"/>
       <c r="G99" s="31"/>
@@ -8295,7 +8255,7 @@
       <c r="A100" s="73"/>
       <c r="B100" s="46"/>
       <c r="C100" s="31"/>
-      <c r="D100" s="71"/>
+      <c r="D100" s="68"/>
       <c r="E100" s="46"/>
       <c r="F100" s="31"/>
       <c r="G100" s="31"/>
@@ -8306,22 +8266,6 @@
       <c r="L100" s="31"/>
       <c r="M100" s="31"/>
       <c r="N100" s="31"/>
-    </row>
-    <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="74"/>
-      <c r="B101" s="46"/>
-      <c r="C101" s="31"/>
-      <c r="D101" s="71"/>
-      <c r="E101" s="46"/>
-      <c r="F101" s="31"/>
-      <c r="G101" s="31"/>
-      <c r="H101" s="31"/>
-      <c r="I101" s="31"/>
-      <c r="J101" s="31"/>
-      <c r="K101" s="31"/>
-      <c r="L101" s="31"/>
-      <c r="M101" s="31"/>
-      <c r="N101" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Removing CO allocation from spreadsheet template (#6316)
Connects #6303 
### Description
This PR removes CO allocations from the spreadsheet template and import

### Testing Plan
1. Download template and confirm Central Office is removed from the allocation sheet
1. Confirm test suite passes
</commit_message>
<xml_diff>
--- a/spec/support/allocationDuplicateRo.xlsx
+++ b/spec/support/allocationDuplicateRo.xlsx
@@ -7,13 +7,13 @@
   <sheets>
     <sheet name="RO Non-Availability Dates" sheetId="1" r:id="rId4"/>
     <sheet name="Board Non-Availability Dates" sheetId="2" r:id="rId5"/>
-    <sheet name="RO &amp; CO Hearing Allocation" sheetId="3" r:id="rId6"/>
+    <sheet name="RO Allocations" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="125">
   <si>
     <t>Example</t>
   </si>
@@ -381,13 +381,10 @@
     <t>Board Non-Availability Dates and Holidays in Date Range</t>
   </si>
   <si>
-    <t>Allocation of Regional Office Video Hearings and Central Office Hearings</t>
+    <t>Allocation of Regional Office Video Hearings</t>
   </si>
   <si>
     <t>Number of Hearing Days Allocated in Date Range</t>
-  </si>
-  <si>
-    <t>Central Office</t>
   </si>
   <si>
     <t xml:space="preserve">Des Moines, IA </t>
@@ -532,7 +529,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -911,49 +908,6 @@
         <color indexed="12"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
@@ -971,7 +925,9 @@
       <right style="thin">
         <color indexed="8"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -998,6 +954,17 @@
         <color indexed="8"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="12"/>
       </bottom>
@@ -1009,7 +976,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1199,40 +1166,37 @@
     <xf numFmtId="49" fontId="9" fillId="4" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="8" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -6316,7 +6280,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N101"/>
+  <dimension ref="A1:N100"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -6403,14 +6367,16 @@
       <c r="M3" s="31"/>
       <c r="N3" s="31"/>
     </row>
-    <row r="4" ht="30.95" customHeight="1">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="65"/>
       <c r="B4" t="s" s="66">
-        <v>124</v>
-      </c>
-      <c r="C4" s="67"/>
+        <v>63</v>
+      </c>
+      <c r="C4" t="s" s="67">
+        <v>4</v>
+      </c>
       <c r="D4" s="68">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" s="46"/>
       <c r="F4" s="31"/>
@@ -6426,13 +6392,13 @@
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="69"/>
       <c r="B5" t="s" s="66">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s" s="70">
-        <v>4</v>
-      </c>
-      <c r="D5" s="71">
-        <v>4</v>
+        <v>64</v>
+      </c>
+      <c r="C5" t="s" s="67">
+        <v>5</v>
+      </c>
+      <c r="D5" s="68">
+        <v>10</v>
       </c>
       <c r="E5" s="46"/>
       <c r="F5" s="31"/>
@@ -6446,15 +6412,15 @@
       <c r="N5" s="31"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="69"/>
+      <c r="A6" s="70"/>
       <c r="B6" t="s" s="66">
-        <v>64</v>
-      </c>
-      <c r="C6" t="s" s="70">
-        <v>5</v>
-      </c>
-      <c r="D6" s="71">
-        <v>10</v>
+        <v>65</v>
+      </c>
+      <c r="C6" t="s" s="67">
+        <v>6</v>
+      </c>
+      <c r="D6" s="68">
+        <v>11</v>
       </c>
       <c r="E6" s="46"/>
       <c r="F6" s="31"/>
@@ -6468,15 +6434,15 @@
       <c r="N6" s="31"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="72"/>
+      <c r="A7" s="70"/>
       <c r="B7" t="s" s="66">
         <v>65</v>
       </c>
-      <c r="C7" t="s" s="70">
+      <c r="C7" t="s" s="67">
         <v>6</v>
       </c>
-      <c r="D7" s="71">
-        <v>11</v>
+      <c r="D7" s="68">
+        <v>12</v>
       </c>
       <c r="E7" s="46"/>
       <c r="F7" s="31"/>
@@ -6490,15 +6456,15 @@
       <c r="N7" s="31"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="72"/>
+      <c r="A8" s="70"/>
       <c r="B8" t="s" s="66">
-        <v>65</v>
-      </c>
-      <c r="C8" t="s" s="70">
-        <v>6</v>
-      </c>
-      <c r="D8" s="71">
-        <v>12</v>
+        <v>66</v>
+      </c>
+      <c r="C8" t="s" s="67">
+        <v>7</v>
+      </c>
+      <c r="D8" s="68">
+        <v>7</v>
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="31"/>
@@ -6512,15 +6478,15 @@
       <c r="N8" s="31"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="72"/>
+      <c r="A9" s="71"/>
       <c r="B9" t="s" s="66">
-        <v>66</v>
-      </c>
-      <c r="C9" t="s" s="70">
-        <v>7</v>
-      </c>
-      <c r="D9" s="71">
-        <v>7</v>
+        <v>67</v>
+      </c>
+      <c r="C9" t="s" s="67">
+        <v>8</v>
+      </c>
+      <c r="D9" s="68">
+        <v>4</v>
       </c>
       <c r="E9" s="46"/>
       <c r="F9" s="31"/>
@@ -6534,15 +6500,15 @@
       <c r="N9" s="31"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="73"/>
+      <c r="A10" s="71"/>
       <c r="B10" t="s" s="66">
-        <v>67</v>
-      </c>
-      <c r="C10" t="s" s="70">
-        <v>8</v>
-      </c>
-      <c r="D10" s="71">
-        <v>4</v>
+        <v>68</v>
+      </c>
+      <c r="C10" t="s" s="67">
+        <v>9</v>
+      </c>
+      <c r="D10" s="68">
+        <v>6</v>
       </c>
       <c r="E10" s="46"/>
       <c r="F10" s="31"/>
@@ -6556,15 +6522,15 @@
       <c r="N10" s="31"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="73"/>
+      <c r="A11" s="71"/>
       <c r="B11" t="s" s="66">
-        <v>68</v>
-      </c>
-      <c r="C11" t="s" s="70">
-        <v>9</v>
-      </c>
-      <c r="D11" s="71">
-        <v>6</v>
+        <v>69</v>
+      </c>
+      <c r="C11" t="s" s="67">
+        <v>10</v>
+      </c>
+      <c r="D11" s="68">
+        <v>3</v>
       </c>
       <c r="E11" s="46"/>
       <c r="F11" s="31"/>
@@ -6578,15 +6544,15 @@
       <c r="N11" s="31"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="73"/>
+      <c r="A12" s="71"/>
       <c r="B12" t="s" s="66">
-        <v>69</v>
-      </c>
-      <c r="C12" t="s" s="70">
-        <v>10</v>
-      </c>
-      <c r="D12" s="71">
-        <v>3</v>
+        <v>70</v>
+      </c>
+      <c r="C12" t="s" s="67">
+        <v>11</v>
+      </c>
+      <c r="D12" s="68">
+        <v>1</v>
       </c>
       <c r="E12" s="46"/>
       <c r="F12" s="31"/>
@@ -6600,15 +6566,15 @@
       <c r="N12" s="31"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="73"/>
+      <c r="A13" s="71"/>
       <c r="B13" t="s" s="66">
-        <v>70</v>
-      </c>
-      <c r="C13" t="s" s="70">
-        <v>11</v>
-      </c>
-      <c r="D13" s="71">
-        <v>1</v>
+        <v>71</v>
+      </c>
+      <c r="C13" t="s" s="67">
+        <v>12</v>
+      </c>
+      <c r="D13" s="68">
+        <v>6</v>
       </c>
       <c r="E13" s="46"/>
       <c r="F13" s="31"/>
@@ -6622,15 +6588,15 @@
       <c r="N13" s="31"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="73"/>
+      <c r="A14" s="71"/>
       <c r="B14" t="s" s="66">
-        <v>71</v>
-      </c>
-      <c r="C14" t="s" s="70">
-        <v>12</v>
-      </c>
-      <c r="D14" s="71">
-        <v>6</v>
+        <v>72</v>
+      </c>
+      <c r="C14" t="s" s="67">
+        <v>13</v>
+      </c>
+      <c r="D14" s="68">
+        <v>8</v>
       </c>
       <c r="E14" s="46"/>
       <c r="F14" s="31"/>
@@ -6644,15 +6610,15 @@
       <c r="N14" s="31"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="73"/>
+      <c r="A15" s="71"/>
       <c r="B15" t="s" s="66">
-        <v>72</v>
-      </c>
-      <c r="C15" t="s" s="70">
-        <v>13</v>
-      </c>
-      <c r="D15" s="71">
-        <v>8</v>
+        <v>73</v>
+      </c>
+      <c r="C15" t="s" s="67">
+        <v>14</v>
+      </c>
+      <c r="D15" s="68">
+        <v>9</v>
       </c>
       <c r="E15" s="46"/>
       <c r="F15" s="31"/>
@@ -6666,15 +6632,15 @@
       <c r="N15" s="31"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="73"/>
+      <c r="A16" s="71"/>
       <c r="B16" t="s" s="66">
-        <v>73</v>
-      </c>
-      <c r="C16" t="s" s="70">
-        <v>14</v>
-      </c>
-      <c r="D16" s="71">
-        <v>9</v>
+        <v>74</v>
+      </c>
+      <c r="C16" t="s" s="67">
+        <v>15</v>
+      </c>
+      <c r="D16" s="68">
+        <v>5</v>
       </c>
       <c r="E16" s="46"/>
       <c r="F16" s="31"/>
@@ -6688,15 +6654,15 @@
       <c r="N16" s="31"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="73"/>
+      <c r="A17" s="71"/>
       <c r="B17" t="s" s="66">
-        <v>74</v>
-      </c>
-      <c r="C17" t="s" s="70">
-        <v>15</v>
-      </c>
-      <c r="D17" s="71">
-        <v>5</v>
+        <v>75</v>
+      </c>
+      <c r="C17" t="s" s="67">
+        <v>16</v>
+      </c>
+      <c r="D17" s="68">
+        <v>4</v>
       </c>
       <c r="E17" s="46"/>
       <c r="F17" s="31"/>
@@ -6710,15 +6676,15 @@
       <c r="N17" s="31"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="73"/>
+      <c r="A18" s="71"/>
       <c r="B18" t="s" s="66">
-        <v>75</v>
-      </c>
-      <c r="C18" t="s" s="70">
-        <v>16</v>
-      </c>
-      <c r="D18" s="71">
-        <v>4</v>
+        <v>76</v>
+      </c>
+      <c r="C18" t="s" s="67">
+        <v>17</v>
+      </c>
+      <c r="D18" s="68">
+        <v>2</v>
       </c>
       <c r="E18" s="46"/>
       <c r="F18" s="31"/>
@@ -6732,15 +6698,15 @@
       <c r="N18" s="31"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="73"/>
+      <c r="A19" s="71"/>
       <c r="B19" t="s" s="66">
-        <v>76</v>
-      </c>
-      <c r="C19" t="s" s="70">
-        <v>17</v>
-      </c>
-      <c r="D19" s="71">
-        <v>2</v>
+        <v>77</v>
+      </c>
+      <c r="C19" t="s" s="67">
+        <v>18</v>
+      </c>
+      <c r="D19" s="68">
+        <v>5</v>
       </c>
       <c r="E19" s="46"/>
       <c r="F19" s="31"/>
@@ -6754,15 +6720,15 @@
       <c r="N19" s="31"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="73"/>
+      <c r="A20" s="71"/>
       <c r="B20" t="s" s="66">
-        <v>77</v>
-      </c>
-      <c r="C20" t="s" s="70">
-        <v>18</v>
-      </c>
-      <c r="D20" s="71">
-        <v>5</v>
+        <v>78</v>
+      </c>
+      <c r="C20" t="s" s="67">
+        <v>19</v>
+      </c>
+      <c r="D20" s="68">
+        <v>7</v>
       </c>
       <c r="E20" s="46"/>
       <c r="F20" s="31"/>
@@ -6776,15 +6742,15 @@
       <c r="N20" s="31"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="73"/>
+      <c r="A21" s="71"/>
       <c r="B21" t="s" s="66">
-        <v>78</v>
-      </c>
-      <c r="C21" t="s" s="70">
-        <v>19</v>
-      </c>
-      <c r="D21" s="71">
-        <v>7</v>
+        <v>79</v>
+      </c>
+      <c r="C21" t="s" s="67">
+        <v>20</v>
+      </c>
+      <c r="D21" s="68">
+        <v>15</v>
       </c>
       <c r="E21" s="46"/>
       <c r="F21" s="31"/>
@@ -6798,15 +6764,15 @@
       <c r="N21" s="31"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="73"/>
+      <c r="A22" s="71"/>
       <c r="B22" t="s" s="66">
-        <v>79</v>
-      </c>
-      <c r="C22" t="s" s="70">
-        <v>20</v>
-      </c>
-      <c r="D22" s="71">
-        <v>15</v>
+        <v>80</v>
+      </c>
+      <c r="C22" t="s" s="67">
+        <v>21</v>
+      </c>
+      <c r="D22" s="68">
+        <v>3</v>
       </c>
       <c r="E22" s="46"/>
       <c r="F22" s="31"/>
@@ -6820,15 +6786,15 @@
       <c r="N22" s="31"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="73"/>
+      <c r="A23" s="71"/>
       <c r="B23" t="s" s="66">
-        <v>80</v>
-      </c>
-      <c r="C23" t="s" s="70">
-        <v>21</v>
-      </c>
-      <c r="D23" s="71">
-        <v>3</v>
+        <v>81</v>
+      </c>
+      <c r="C23" t="s" s="67">
+        <v>22</v>
+      </c>
+      <c r="D23" s="68">
+        <v>7</v>
       </c>
       <c r="E23" s="46"/>
       <c r="F23" s="31"/>
@@ -6842,15 +6808,15 @@
       <c r="N23" s="31"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="73"/>
+      <c r="A24" s="71"/>
       <c r="B24" t="s" s="66">
-        <v>81</v>
-      </c>
-      <c r="C24" t="s" s="70">
-        <v>22</v>
-      </c>
-      <c r="D24" s="71">
-        <v>7</v>
+        <v>82</v>
+      </c>
+      <c r="C24" t="s" s="67">
+        <v>23</v>
+      </c>
+      <c r="D24" s="68">
+        <v>0</v>
       </c>
       <c r="E24" s="46"/>
       <c r="F24" s="31"/>
@@ -6864,15 +6830,15 @@
       <c r="N24" s="31"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="73"/>
+      <c r="A25" s="71"/>
       <c r="B25" t="s" s="66">
-        <v>82</v>
-      </c>
-      <c r="C25" t="s" s="70">
-        <v>23</v>
-      </c>
-      <c r="D25" s="71">
-        <v>0</v>
+        <v>83</v>
+      </c>
+      <c r="C25" t="s" s="67">
+        <v>24</v>
+      </c>
+      <c r="D25" s="68">
+        <v>3</v>
       </c>
       <c r="E25" s="46"/>
       <c r="F25" s="31"/>
@@ -6886,15 +6852,15 @@
       <c r="N25" s="31"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="73"/>
+      <c r="A26" s="71"/>
       <c r="B26" t="s" s="66">
-        <v>83</v>
-      </c>
-      <c r="C26" t="s" s="70">
-        <v>24</v>
-      </c>
-      <c r="D26" s="71">
-        <v>3</v>
+        <v>84</v>
+      </c>
+      <c r="C26" t="s" s="67">
+        <v>25</v>
+      </c>
+      <c r="D26" s="68">
+        <v>7</v>
       </c>
       <c r="E26" s="46"/>
       <c r="F26" s="31"/>
@@ -6908,15 +6874,15 @@
       <c r="N26" s="31"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="73"/>
+      <c r="A27" s="71"/>
       <c r="B27" t="s" s="66">
-        <v>84</v>
-      </c>
-      <c r="C27" t="s" s="70">
-        <v>25</v>
-      </c>
-      <c r="D27" s="71">
-        <v>7</v>
+        <v>85</v>
+      </c>
+      <c r="C27" t="s" s="67">
+        <v>26</v>
+      </c>
+      <c r="D27" s="68">
+        <v>3</v>
       </c>
       <c r="E27" s="46"/>
       <c r="F27" s="31"/>
@@ -6930,15 +6896,15 @@
       <c r="N27" s="31"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="73"/>
+      <c r="A28" s="71"/>
       <c r="B28" t="s" s="66">
-        <v>85</v>
-      </c>
-      <c r="C28" t="s" s="70">
-        <v>26</v>
-      </c>
-      <c r="D28" s="71">
-        <v>3</v>
+        <v>86</v>
+      </c>
+      <c r="C28" t="s" s="67">
+        <v>27</v>
+      </c>
+      <c r="D28" s="68">
+        <v>2</v>
       </c>
       <c r="E28" s="46"/>
       <c r="F28" s="31"/>
@@ -6952,15 +6918,15 @@
       <c r="N28" s="31"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="73"/>
+      <c r="A29" s="71"/>
       <c r="B29" t="s" s="66">
-        <v>86</v>
-      </c>
-      <c r="C29" t="s" s="70">
-        <v>27</v>
-      </c>
-      <c r="D29" s="71">
-        <v>2</v>
+        <v>87</v>
+      </c>
+      <c r="C29" t="s" s="67">
+        <v>28</v>
+      </c>
+      <c r="D29" s="68">
+        <v>5</v>
       </c>
       <c r="E29" s="46"/>
       <c r="F29" s="31"/>
@@ -6974,15 +6940,15 @@
       <c r="N29" s="31"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="73"/>
+      <c r="A30" s="71"/>
       <c r="B30" t="s" s="66">
-        <v>87</v>
-      </c>
-      <c r="C30" t="s" s="70">
-        <v>28</v>
-      </c>
-      <c r="D30" s="71">
-        <v>5</v>
+        <v>88</v>
+      </c>
+      <c r="C30" t="s" s="67">
+        <v>29</v>
+      </c>
+      <c r="D30" s="68">
+        <v>7</v>
       </c>
       <c r="E30" s="46"/>
       <c r="F30" s="31"/>
@@ -6996,15 +6962,15 @@
       <c r="N30" s="31"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="73"/>
+      <c r="A31" s="71"/>
       <c r="B31" t="s" s="66">
-        <v>88</v>
-      </c>
-      <c r="C31" t="s" s="70">
-        <v>29</v>
-      </c>
-      <c r="D31" s="71">
-        <v>7</v>
+        <v>89</v>
+      </c>
+      <c r="C31" t="s" s="67">
+        <v>30</v>
+      </c>
+      <c r="D31" s="68">
+        <v>4</v>
       </c>
       <c r="E31" s="46"/>
       <c r="F31" s="31"/>
@@ -7018,14 +6984,14 @@
       <c r="N31" s="31"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="73"/>
+      <c r="A32" s="71"/>
       <c r="B32" t="s" s="66">
-        <v>89</v>
-      </c>
-      <c r="C32" t="s" s="70">
-        <v>30</v>
-      </c>
-      <c r="D32" s="71">
+        <v>90</v>
+      </c>
+      <c r="C32" t="s" s="67">
+        <v>31</v>
+      </c>
+      <c r="D32" s="68">
         <v>4</v>
       </c>
       <c r="E32" s="46"/>
@@ -7040,15 +7006,15 @@
       <c r="N32" s="31"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="73"/>
+      <c r="A33" s="71"/>
       <c r="B33" t="s" s="66">
-        <v>90</v>
-      </c>
-      <c r="C33" t="s" s="70">
-        <v>31</v>
-      </c>
-      <c r="D33" s="71">
-        <v>4</v>
+        <v>124</v>
+      </c>
+      <c r="C33" t="s" s="67">
+        <v>32</v>
+      </c>
+      <c r="D33" s="68">
+        <v>2</v>
       </c>
       <c r="E33" s="46"/>
       <c r="F33" s="31"/>
@@ -7062,15 +7028,15 @@
       <c r="N33" s="31"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="73"/>
+      <c r="A34" s="71"/>
       <c r="B34" t="s" s="66">
-        <v>125</v>
-      </c>
-      <c r="C34" t="s" s="70">
-        <v>32</v>
-      </c>
-      <c r="D34" s="71">
-        <v>2</v>
+        <v>92</v>
+      </c>
+      <c r="C34" t="s" s="67">
+        <v>33</v>
+      </c>
+      <c r="D34" s="68">
+        <v>5</v>
       </c>
       <c r="E34" s="46"/>
       <c r="F34" s="31"/>
@@ -7084,15 +7050,15 @@
       <c r="N34" s="31"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="73"/>
+      <c r="A35" s="71"/>
       <c r="B35" t="s" s="66">
-        <v>92</v>
-      </c>
-      <c r="C35" t="s" s="70">
-        <v>33</v>
-      </c>
-      <c r="D35" s="71">
-        <v>5</v>
+        <v>93</v>
+      </c>
+      <c r="C35" t="s" s="67">
+        <v>34</v>
+      </c>
+      <c r="D35" s="68">
+        <v>7</v>
       </c>
       <c r="E35" s="46"/>
       <c r="F35" s="31"/>
@@ -7106,15 +7072,15 @@
       <c r="N35" s="31"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="73"/>
+      <c r="A36" s="71"/>
       <c r="B36" t="s" s="66">
-        <v>93</v>
-      </c>
-      <c r="C36" t="s" s="70">
-        <v>34</v>
-      </c>
-      <c r="D36" s="71">
-        <v>7</v>
+        <v>94</v>
+      </c>
+      <c r="C36" t="s" s="67">
+        <v>35</v>
+      </c>
+      <c r="D36" s="68">
+        <v>9</v>
       </c>
       <c r="E36" s="46"/>
       <c r="F36" s="31"/>
@@ -7128,15 +7094,15 @@
       <c r="N36" s="31"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="73"/>
+      <c r="A37" s="71"/>
       <c r="B37" t="s" s="66">
-        <v>94</v>
-      </c>
-      <c r="C37" t="s" s="70">
-        <v>35</v>
-      </c>
-      <c r="D37" s="71">
-        <v>9</v>
+        <v>95</v>
+      </c>
+      <c r="C37" t="s" s="67">
+        <v>36</v>
+      </c>
+      <c r="D37" s="68">
+        <v>4</v>
       </c>
       <c r="E37" s="46"/>
       <c r="F37" s="31"/>
@@ -7150,15 +7116,15 @@
       <c r="N37" s="31"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="73"/>
+      <c r="A38" s="71"/>
       <c r="B38" t="s" s="66">
-        <v>95</v>
-      </c>
-      <c r="C38" t="s" s="70">
-        <v>36</v>
-      </c>
-      <c r="D38" s="71">
-        <v>4</v>
+        <v>96</v>
+      </c>
+      <c r="C38" t="s" s="67">
+        <v>37</v>
+      </c>
+      <c r="D38" s="68">
+        <v>2</v>
       </c>
       <c r="E38" s="46"/>
       <c r="F38" s="31"/>
@@ -7172,15 +7138,15 @@
       <c r="N38" s="31"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="73"/>
+      <c r="A39" s="71"/>
       <c r="B39" t="s" s="66">
-        <v>96</v>
-      </c>
-      <c r="C39" t="s" s="70">
-        <v>37</v>
-      </c>
-      <c r="D39" s="71">
-        <v>2</v>
+        <v>97</v>
+      </c>
+      <c r="C39" t="s" s="67">
+        <v>38</v>
+      </c>
+      <c r="D39" s="68">
+        <v>6</v>
       </c>
       <c r="E39" s="46"/>
       <c r="F39" s="31"/>
@@ -7194,15 +7160,15 @@
       <c r="N39" s="31"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="73"/>
+      <c r="A40" s="71"/>
       <c r="B40" t="s" s="66">
-        <v>97</v>
-      </c>
-      <c r="C40" t="s" s="70">
-        <v>38</v>
-      </c>
-      <c r="D40" s="71">
-        <v>6</v>
+        <v>98</v>
+      </c>
+      <c r="C40" t="s" s="67">
+        <v>39</v>
+      </c>
+      <c r="D40" s="68">
+        <v>3</v>
       </c>
       <c r="E40" s="46"/>
       <c r="F40" s="31"/>
@@ -7216,15 +7182,15 @@
       <c r="N40" s="31"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="73"/>
+      <c r="A41" s="71"/>
       <c r="B41" t="s" s="66">
-        <v>98</v>
-      </c>
-      <c r="C41" t="s" s="70">
-        <v>39</v>
-      </c>
-      <c r="D41" s="71">
-        <v>3</v>
+        <v>99</v>
+      </c>
+      <c r="C41" t="s" s="67">
+        <v>40</v>
+      </c>
+      <c r="D41" s="68">
+        <v>2</v>
       </c>
       <c r="E41" s="46"/>
       <c r="F41" s="31"/>
@@ -7238,15 +7204,15 @@
       <c r="N41" s="31"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="73"/>
+      <c r="A42" s="71"/>
       <c r="B42" t="s" s="66">
-        <v>99</v>
-      </c>
-      <c r="C42" t="s" s="70">
-        <v>40</v>
-      </c>
-      <c r="D42" s="71">
-        <v>2</v>
+        <v>100</v>
+      </c>
+      <c r="C42" t="s" s="67">
+        <v>41</v>
+      </c>
+      <c r="D42" s="68">
+        <v>6</v>
       </c>
       <c r="E42" s="46"/>
       <c r="F42" s="31"/>
@@ -7260,15 +7226,15 @@
       <c r="N42" s="31"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="73"/>
+      <c r="A43" s="71"/>
       <c r="B43" t="s" s="66">
-        <v>100</v>
-      </c>
-      <c r="C43" t="s" s="70">
-        <v>41</v>
-      </c>
-      <c r="D43" s="71">
-        <v>6</v>
+        <v>101</v>
+      </c>
+      <c r="C43" t="s" s="67">
+        <v>42</v>
+      </c>
+      <c r="D43" s="68">
+        <v>5</v>
       </c>
       <c r="E43" s="46"/>
       <c r="F43" s="31"/>
@@ -7282,15 +7248,15 @@
       <c r="N43" s="31"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="73"/>
+      <c r="A44" s="71"/>
       <c r="B44" t="s" s="66">
-        <v>101</v>
-      </c>
-      <c r="C44" t="s" s="70">
-        <v>42</v>
-      </c>
-      <c r="D44" s="71">
-        <v>5</v>
+        <v>102</v>
+      </c>
+      <c r="C44" t="s" s="67">
+        <v>43</v>
+      </c>
+      <c r="D44" s="68">
+        <v>3</v>
       </c>
       <c r="E44" s="46"/>
       <c r="F44" s="31"/>
@@ -7304,15 +7270,15 @@
       <c r="N44" s="31"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="73"/>
+      <c r="A45" s="71"/>
       <c r="B45" t="s" s="66">
-        <v>102</v>
-      </c>
-      <c r="C45" t="s" s="70">
-        <v>43</v>
-      </c>
-      <c r="D45" s="71">
-        <v>3</v>
+        <v>103</v>
+      </c>
+      <c r="C45" t="s" s="67">
+        <v>44</v>
+      </c>
+      <c r="D45" s="68">
+        <v>5</v>
       </c>
       <c r="E45" s="46"/>
       <c r="F45" s="31"/>
@@ -7326,15 +7292,15 @@
       <c r="N45" s="31"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="73"/>
+      <c r="A46" s="71"/>
       <c r="B46" t="s" s="66">
-        <v>103</v>
-      </c>
-      <c r="C46" t="s" s="70">
-        <v>44</v>
-      </c>
-      <c r="D46" s="71">
-        <v>5</v>
+        <v>104</v>
+      </c>
+      <c r="C46" t="s" s="67">
+        <v>45</v>
+      </c>
+      <c r="D46" s="68">
+        <v>36</v>
       </c>
       <c r="E46" s="46"/>
       <c r="F46" s="31"/>
@@ -7348,15 +7314,15 @@
       <c r="N46" s="31"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="73"/>
+      <c r="A47" s="71"/>
       <c r="B47" t="s" s="66">
-        <v>104</v>
-      </c>
-      <c r="C47" t="s" s="70">
-        <v>45</v>
-      </c>
-      <c r="D47" s="71">
-        <v>36</v>
+        <v>105</v>
+      </c>
+      <c r="C47" t="s" s="67">
+        <v>46</v>
+      </c>
+      <c r="D47" s="68">
+        <v>7</v>
       </c>
       <c r="E47" s="46"/>
       <c r="F47" s="31"/>
@@ -7370,15 +7336,15 @@
       <c r="N47" s="31"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="73"/>
+      <c r="A48" s="71"/>
       <c r="B48" t="s" s="66">
-        <v>105</v>
-      </c>
-      <c r="C48" t="s" s="70">
-        <v>46</v>
-      </c>
-      <c r="D48" s="71">
-        <v>7</v>
+        <v>106</v>
+      </c>
+      <c r="C48" t="s" s="67">
+        <v>47</v>
+      </c>
+      <c r="D48" s="68">
+        <v>1</v>
       </c>
       <c r="E48" s="46"/>
       <c r="F48" s="31"/>
@@ -7392,15 +7358,15 @@
       <c r="N48" s="31"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="73"/>
+      <c r="A49" s="71"/>
       <c r="B49" t="s" s="66">
-        <v>106</v>
-      </c>
-      <c r="C49" t="s" s="70">
-        <v>47</v>
-      </c>
-      <c r="D49" s="71">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="C49" t="s" s="67">
+        <v>48</v>
+      </c>
+      <c r="D49" s="68">
+        <v>4</v>
       </c>
       <c r="E49" s="46"/>
       <c r="F49" s="31"/>
@@ -7414,15 +7380,15 @@
       <c r="N49" s="31"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="73"/>
+      <c r="A50" s="71"/>
       <c r="B50" t="s" s="66">
-        <v>107</v>
-      </c>
-      <c r="C50" t="s" s="70">
-        <v>48</v>
-      </c>
-      <c r="D50" s="71">
-        <v>4</v>
+        <v>108</v>
+      </c>
+      <c r="C50" t="s" s="67">
+        <v>49</v>
+      </c>
+      <c r="D50" s="68">
+        <v>57</v>
       </c>
       <c r="E50" s="46"/>
       <c r="F50" s="31"/>
@@ -7436,15 +7402,15 @@
       <c r="N50" s="31"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="73"/>
+      <c r="A51" s="71"/>
       <c r="B51" t="s" s="66">
-        <v>108</v>
-      </c>
-      <c r="C51" t="s" s="70">
-        <v>49</v>
-      </c>
-      <c r="D51" s="71">
-        <v>57</v>
+        <v>109</v>
+      </c>
+      <c r="C51" t="s" s="67">
+        <v>50</v>
+      </c>
+      <c r="D51" s="68">
+        <v>3</v>
       </c>
       <c r="E51" s="46"/>
       <c r="F51" s="31"/>
@@ -7458,15 +7424,15 @@
       <c r="N51" s="31"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="73"/>
+      <c r="A52" s="71"/>
       <c r="B52" t="s" s="66">
-        <v>109</v>
-      </c>
-      <c r="C52" t="s" s="70">
-        <v>50</v>
-      </c>
-      <c r="D52" s="71">
-        <v>3</v>
+        <v>110</v>
+      </c>
+      <c r="C52" t="s" s="67">
+        <v>51</v>
+      </c>
+      <c r="D52" s="68">
+        <v>1</v>
       </c>
       <c r="E52" s="46"/>
       <c r="F52" s="31"/>
@@ -7480,15 +7446,15 @@
       <c r="N52" s="31"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="73"/>
+      <c r="A53" s="71"/>
       <c r="B53" t="s" s="66">
-        <v>110</v>
-      </c>
-      <c r="C53" t="s" s="70">
-        <v>51</v>
-      </c>
-      <c r="D53" s="71">
-        <v>1</v>
+        <v>111</v>
+      </c>
+      <c r="C53" t="s" s="67">
+        <v>52</v>
+      </c>
+      <c r="D53" s="68">
+        <v>7</v>
       </c>
       <c r="E53" s="46"/>
       <c r="F53" s="31"/>
@@ -7502,15 +7468,15 @@
       <c r="N53" s="31"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="73"/>
+      <c r="A54" s="71"/>
       <c r="B54" t="s" s="66">
-        <v>111</v>
-      </c>
-      <c r="C54" t="s" s="70">
-        <v>52</v>
-      </c>
-      <c r="D54" s="71">
-        <v>7</v>
+        <v>112</v>
+      </c>
+      <c r="C54" t="s" s="67">
+        <v>53</v>
+      </c>
+      <c r="D54" s="68">
+        <v>4</v>
       </c>
       <c r="E54" s="46"/>
       <c r="F54" s="31"/>
@@ -7524,15 +7490,15 @@
       <c r="N54" s="31"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="73"/>
+      <c r="A55" s="71"/>
       <c r="B55" t="s" s="66">
-        <v>112</v>
-      </c>
-      <c r="C55" t="s" s="70">
-        <v>53</v>
-      </c>
-      <c r="D55" s="71">
-        <v>4</v>
+        <v>113</v>
+      </c>
+      <c r="C55" t="s" s="67">
+        <v>54</v>
+      </c>
+      <c r="D55" s="68">
+        <v>2</v>
       </c>
       <c r="E55" s="46"/>
       <c r="F55" s="31"/>
@@ -7546,15 +7512,15 @@
       <c r="N55" s="31"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="73"/>
+      <c r="A56" s="71"/>
       <c r="B56" t="s" s="66">
-        <v>113</v>
-      </c>
-      <c r="C56" t="s" s="70">
-        <v>54</v>
-      </c>
-      <c r="D56" s="71">
-        <v>2</v>
+        <v>114</v>
+      </c>
+      <c r="C56" t="s" s="67">
+        <v>55</v>
+      </c>
+      <c r="D56" s="68">
+        <v>6</v>
       </c>
       <c r="E56" s="46"/>
       <c r="F56" s="31"/>
@@ -7568,15 +7534,15 @@
       <c r="N56" s="31"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="73"/>
+      <c r="A57" s="71"/>
       <c r="B57" t="s" s="66">
-        <v>114</v>
-      </c>
-      <c r="C57" t="s" s="70">
-        <v>55</v>
-      </c>
-      <c r="D57" s="71">
-        <v>6</v>
+        <v>115</v>
+      </c>
+      <c r="C57" t="s" s="67">
+        <v>56</v>
+      </c>
+      <c r="D57" s="68">
+        <v>8</v>
       </c>
       <c r="E57" s="46"/>
       <c r="F57" s="31"/>
@@ -7590,15 +7556,15 @@
       <c r="N57" s="31"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="73"/>
+      <c r="A58" s="71"/>
       <c r="B58" t="s" s="66">
-        <v>115</v>
-      </c>
-      <c r="C58" t="s" s="70">
-        <v>56</v>
-      </c>
-      <c r="D58" s="71">
-        <v>8</v>
+        <v>116</v>
+      </c>
+      <c r="C58" t="s" s="67">
+        <v>57</v>
+      </c>
+      <c r="D58" s="68">
+        <v>2</v>
       </c>
       <c r="E58" s="46"/>
       <c r="F58" s="31"/>
@@ -7612,14 +7578,14 @@
       <c r="N58" s="31"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="73"/>
+      <c r="A59" s="71"/>
       <c r="B59" t="s" s="66">
-        <v>116</v>
-      </c>
-      <c r="C59" t="s" s="70">
-        <v>57</v>
-      </c>
-      <c r="D59" s="71">
+        <v>117</v>
+      </c>
+      <c r="C59" t="s" s="67">
+        <v>58</v>
+      </c>
+      <c r="D59" s="68">
         <v>2</v>
       </c>
       <c r="E59" s="46"/>
@@ -7634,15 +7600,15 @@
       <c r="N59" s="31"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="73"/>
+      <c r="A60" s="71"/>
       <c r="B60" t="s" s="66">
-        <v>117</v>
-      </c>
-      <c r="C60" t="s" s="70">
-        <v>58</v>
-      </c>
-      <c r="D60" s="71">
-        <v>2</v>
+        <v>118</v>
+      </c>
+      <c r="C60" t="s" s="67">
+        <v>59</v>
+      </c>
+      <c r="D60" s="68">
+        <v>6</v>
       </c>
       <c r="E60" s="46"/>
       <c r="F60" s="31"/>
@@ -7656,15 +7622,15 @@
       <c r="N60" s="31"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="73"/>
+      <c r="A61" s="71"/>
       <c r="B61" t="s" s="66">
-        <v>118</v>
-      </c>
-      <c r="C61" t="s" s="70">
-        <v>59</v>
-      </c>
-      <c r="D61" s="71">
-        <v>6</v>
+        <v>119</v>
+      </c>
+      <c r="C61" t="s" s="67">
+        <v>60</v>
+      </c>
+      <c r="D61" s="68">
+        <v>1</v>
       </c>
       <c r="E61" s="46"/>
       <c r="F61" s="31"/>
@@ -7678,16 +7644,10 @@
       <c r="N61" s="31"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="73"/>
-      <c r="B62" t="s" s="66">
-        <v>119</v>
-      </c>
-      <c r="C62" t="s" s="70">
-        <v>60</v>
-      </c>
-      <c r="D62" s="71">
-        <v>1</v>
-      </c>
+      <c r="A62" s="71"/>
+      <c r="B62" s="72"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="68"/>
       <c r="E62" s="46"/>
       <c r="F62" s="31"/>
       <c r="G62" s="31"/>
@@ -7700,10 +7660,10 @@
       <c r="N62" s="31"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="73"/>
-      <c r="B63" s="67"/>
+      <c r="A63" s="71"/>
+      <c r="B63" s="46"/>
       <c r="C63" s="31"/>
-      <c r="D63" s="71"/>
+      <c r="D63" s="68"/>
       <c r="E63" s="46"/>
       <c r="F63" s="31"/>
       <c r="G63" s="31"/>
@@ -7716,10 +7676,10 @@
       <c r="N63" s="31"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="73"/>
+      <c r="A64" s="71"/>
       <c r="B64" s="46"/>
       <c r="C64" s="31"/>
-      <c r="D64" s="71"/>
+      <c r="D64" s="68"/>
       <c r="E64" s="46"/>
       <c r="F64" s="31"/>
       <c r="G64" s="31"/>
@@ -7732,10 +7692,10 @@
       <c r="N64" s="31"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="73"/>
+      <c r="A65" s="71"/>
       <c r="B65" s="46"/>
       <c r="C65" s="31"/>
-      <c r="D65" s="71"/>
+      <c r="D65" s="68"/>
       <c r="E65" s="46"/>
       <c r="F65" s="31"/>
       <c r="G65" s="31"/>
@@ -7748,10 +7708,10 @@
       <c r="N65" s="31"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="73"/>
+      <c r="A66" s="71"/>
       <c r="B66" s="46"/>
       <c r="C66" s="31"/>
-      <c r="D66" s="71"/>
+      <c r="D66" s="68"/>
       <c r="E66" s="46"/>
       <c r="F66" s="31"/>
       <c r="G66" s="31"/>
@@ -7764,10 +7724,10 @@
       <c r="N66" s="31"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="73"/>
+      <c r="A67" s="71"/>
       <c r="B67" s="46"/>
       <c r="C67" s="31"/>
-      <c r="D67" s="71"/>
+      <c r="D67" s="68"/>
       <c r="E67" s="46"/>
       <c r="F67" s="31"/>
       <c r="G67" s="31"/>
@@ -7780,10 +7740,10 @@
       <c r="N67" s="31"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="73"/>
+      <c r="A68" s="71"/>
       <c r="B68" s="46"/>
       <c r="C68" s="31"/>
-      <c r="D68" s="71"/>
+      <c r="D68" s="68"/>
       <c r="E68" s="46"/>
       <c r="F68" s="31"/>
       <c r="G68" s="31"/>
@@ -7796,10 +7756,10 @@
       <c r="N68" s="31"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="73"/>
+      <c r="A69" s="71"/>
       <c r="B69" s="46"/>
       <c r="C69" s="31"/>
-      <c r="D69" s="71"/>
+      <c r="D69" s="68"/>
       <c r="E69" s="46"/>
       <c r="F69" s="31"/>
       <c r="G69" s="31"/>
@@ -7812,10 +7772,10 @@
       <c r="N69" s="31"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="73"/>
+      <c r="A70" s="71"/>
       <c r="B70" s="46"/>
       <c r="C70" s="31"/>
-      <c r="D70" s="71"/>
+      <c r="D70" s="68"/>
       <c r="E70" s="46"/>
       <c r="F70" s="31"/>
       <c r="G70" s="31"/>
@@ -7828,10 +7788,10 @@
       <c r="N70" s="31"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="73"/>
+      <c r="A71" s="71"/>
       <c r="B71" s="46"/>
       <c r="C71" s="31"/>
-      <c r="D71" s="71"/>
+      <c r="D71" s="68"/>
       <c r="E71" s="46"/>
       <c r="F71" s="31"/>
       <c r="G71" s="31"/>
@@ -7844,10 +7804,10 @@
       <c r="N71" s="31"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="73"/>
+      <c r="A72" s="71"/>
       <c r="B72" s="46"/>
       <c r="C72" s="31"/>
-      <c r="D72" s="71"/>
+      <c r="D72" s="68"/>
       <c r="E72" s="46"/>
       <c r="F72" s="31"/>
       <c r="G72" s="31"/>
@@ -7860,10 +7820,10 @@
       <c r="N72" s="31"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="73"/>
+      <c r="A73" s="71"/>
       <c r="B73" s="46"/>
       <c r="C73" s="31"/>
-      <c r="D73" s="71"/>
+      <c r="D73" s="68"/>
       <c r="E73" s="46"/>
       <c r="F73" s="31"/>
       <c r="G73" s="31"/>
@@ -7876,10 +7836,10 @@
       <c r="N73" s="31"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="73"/>
+      <c r="A74" s="71"/>
       <c r="B74" s="46"/>
       <c r="C74" s="31"/>
-      <c r="D74" s="71"/>
+      <c r="D74" s="68"/>
       <c r="E74" s="46"/>
       <c r="F74" s="31"/>
       <c r="G74" s="31"/>
@@ -7892,10 +7852,10 @@
       <c r="N74" s="31"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="73"/>
+      <c r="A75" s="71"/>
       <c r="B75" s="46"/>
       <c r="C75" s="31"/>
-      <c r="D75" s="71"/>
+      <c r="D75" s="68"/>
       <c r="E75" s="46"/>
       <c r="F75" s="31"/>
       <c r="G75" s="31"/>
@@ -7908,10 +7868,10 @@
       <c r="N75" s="31"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="73"/>
+      <c r="A76" s="71"/>
       <c r="B76" s="46"/>
       <c r="C76" s="31"/>
-      <c r="D76" s="71"/>
+      <c r="D76" s="68"/>
       <c r="E76" s="46"/>
       <c r="F76" s="31"/>
       <c r="G76" s="31"/>
@@ -7924,10 +7884,10 @@
       <c r="N76" s="31"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="73"/>
+      <c r="A77" s="71"/>
       <c r="B77" s="46"/>
       <c r="C77" s="31"/>
-      <c r="D77" s="71"/>
+      <c r="D77" s="68"/>
       <c r="E77" s="46"/>
       <c r="F77" s="31"/>
       <c r="G77" s="31"/>
@@ -7940,10 +7900,10 @@
       <c r="N77" s="31"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="73"/>
+      <c r="A78" s="71"/>
       <c r="B78" s="46"/>
       <c r="C78" s="31"/>
-      <c r="D78" s="71"/>
+      <c r="D78" s="68"/>
       <c r="E78" s="46"/>
       <c r="F78" s="31"/>
       <c r="G78" s="31"/>
@@ -7956,10 +7916,10 @@
       <c r="N78" s="31"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="73"/>
+      <c r="A79" s="71"/>
       <c r="B79" s="46"/>
       <c r="C79" s="31"/>
-      <c r="D79" s="71"/>
+      <c r="D79" s="68"/>
       <c r="E79" s="46"/>
       <c r="F79" s="31"/>
       <c r="G79" s="31"/>
@@ -7972,10 +7932,10 @@
       <c r="N79" s="31"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="73"/>
+      <c r="A80" s="71"/>
       <c r="B80" s="46"/>
       <c r="C80" s="31"/>
-      <c r="D80" s="71"/>
+      <c r="D80" s="68"/>
       <c r="E80" s="46"/>
       <c r="F80" s="31"/>
       <c r="G80" s="31"/>
@@ -7988,10 +7948,10 @@
       <c r="N80" s="31"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="73"/>
+      <c r="A81" s="71"/>
       <c r="B81" s="46"/>
       <c r="C81" s="31"/>
-      <c r="D81" s="71"/>
+      <c r="D81" s="68"/>
       <c r="E81" s="46"/>
       <c r="F81" s="31"/>
       <c r="G81" s="31"/>
@@ -8004,10 +7964,10 @@
       <c r="N81" s="31"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="73"/>
+      <c r="A82" s="71"/>
       <c r="B82" s="46"/>
       <c r="C82" s="31"/>
-      <c r="D82" s="71"/>
+      <c r="D82" s="68"/>
       <c r="E82" s="46"/>
       <c r="F82" s="31"/>
       <c r="G82" s="31"/>
@@ -8020,10 +7980,10 @@
       <c r="N82" s="31"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="73"/>
+      <c r="A83" s="71"/>
       <c r="B83" s="46"/>
       <c r="C83" s="31"/>
-      <c r="D83" s="71"/>
+      <c r="D83" s="68"/>
       <c r="E83" s="46"/>
       <c r="F83" s="31"/>
       <c r="G83" s="31"/>
@@ -8036,10 +7996,10 @@
       <c r="N83" s="31"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="73"/>
+      <c r="A84" s="71"/>
       <c r="B84" s="46"/>
       <c r="C84" s="31"/>
-      <c r="D84" s="71"/>
+      <c r="D84" s="68"/>
       <c r="E84" s="46"/>
       <c r="F84" s="31"/>
       <c r="G84" s="31"/>
@@ -8052,10 +8012,10 @@
       <c r="N84" s="31"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="73"/>
+      <c r="A85" s="71"/>
       <c r="B85" s="46"/>
       <c r="C85" s="31"/>
-      <c r="D85" s="71"/>
+      <c r="D85" s="68"/>
       <c r="E85" s="46"/>
       <c r="F85" s="31"/>
       <c r="G85" s="31"/>
@@ -8068,10 +8028,10 @@
       <c r="N85" s="31"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="73"/>
+      <c r="A86" s="71"/>
       <c r="B86" s="46"/>
       <c r="C86" s="31"/>
-      <c r="D86" s="71"/>
+      <c r="D86" s="68"/>
       <c r="E86" s="46"/>
       <c r="F86" s="31"/>
       <c r="G86" s="31"/>
@@ -8084,10 +8044,10 @@
       <c r="N86" s="31"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="73"/>
+      <c r="A87" s="71"/>
       <c r="B87" s="46"/>
       <c r="C87" s="31"/>
-      <c r="D87" s="71"/>
+      <c r="D87" s="68"/>
       <c r="E87" s="46"/>
       <c r="F87" s="31"/>
       <c r="G87" s="31"/>
@@ -8100,10 +8060,10 @@
       <c r="N87" s="31"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="73"/>
+      <c r="A88" s="71"/>
       <c r="B88" s="46"/>
       <c r="C88" s="31"/>
-      <c r="D88" s="71"/>
+      <c r="D88" s="68"/>
       <c r="E88" s="46"/>
       <c r="F88" s="31"/>
       <c r="G88" s="31"/>
@@ -8116,10 +8076,10 @@
       <c r="N88" s="31"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="73"/>
+      <c r="A89" s="71"/>
       <c r="B89" s="46"/>
       <c r="C89" s="31"/>
-      <c r="D89" s="71"/>
+      <c r="D89" s="68"/>
       <c r="E89" s="46"/>
       <c r="F89" s="31"/>
       <c r="G89" s="31"/>
@@ -8132,10 +8092,10 @@
       <c r="N89" s="31"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="73"/>
+      <c r="A90" s="71"/>
       <c r="B90" s="46"/>
       <c r="C90" s="31"/>
-      <c r="D90" s="71"/>
+      <c r="D90" s="68"/>
       <c r="E90" s="46"/>
       <c r="F90" s="31"/>
       <c r="G90" s="31"/>
@@ -8148,10 +8108,10 @@
       <c r="N90" s="31"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="73"/>
+      <c r="A91" s="71"/>
       <c r="B91" s="46"/>
       <c r="C91" s="31"/>
-      <c r="D91" s="71"/>
+      <c r="D91" s="68"/>
       <c r="E91" s="46"/>
       <c r="F91" s="31"/>
       <c r="G91" s="31"/>
@@ -8164,10 +8124,10 @@
       <c r="N91" s="31"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="73"/>
+      <c r="A92" s="71"/>
       <c r="B92" s="46"/>
       <c r="C92" s="31"/>
-      <c r="D92" s="71"/>
+      <c r="D92" s="68"/>
       <c r="E92" s="46"/>
       <c r="F92" s="31"/>
       <c r="G92" s="31"/>
@@ -8180,10 +8140,10 @@
       <c r="N92" s="31"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="73"/>
+      <c r="A93" s="71"/>
       <c r="B93" s="46"/>
       <c r="C93" s="31"/>
-      <c r="D93" s="71"/>
+      <c r="D93" s="68"/>
       <c r="E93" s="46"/>
       <c r="F93" s="31"/>
       <c r="G93" s="31"/>
@@ -8196,10 +8156,10 @@
       <c r="N93" s="31"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="73"/>
+      <c r="A94" s="71"/>
       <c r="B94" s="46"/>
       <c r="C94" s="31"/>
-      <c r="D94" s="71"/>
+      <c r="D94" s="68"/>
       <c r="E94" s="46"/>
       <c r="F94" s="31"/>
       <c r="G94" s="31"/>
@@ -8212,10 +8172,10 @@
       <c r="N94" s="31"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="73"/>
+      <c r="A95" s="71"/>
       <c r="B95" s="46"/>
       <c r="C95" s="31"/>
-      <c r="D95" s="71"/>
+      <c r="D95" s="68"/>
       <c r="E95" s="46"/>
       <c r="F95" s="31"/>
       <c r="G95" s="31"/>
@@ -8228,10 +8188,10 @@
       <c r="N95" s="31"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="73"/>
+      <c r="A96" s="71"/>
       <c r="B96" s="46"/>
       <c r="C96" s="31"/>
-      <c r="D96" s="71"/>
+      <c r="D96" s="68"/>
       <c r="E96" s="46"/>
       <c r="F96" s="31"/>
       <c r="G96" s="31"/>
@@ -8244,10 +8204,10 @@
       <c r="N96" s="31"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="73"/>
+      <c r="A97" s="71"/>
       <c r="B97" s="46"/>
       <c r="C97" s="31"/>
-      <c r="D97" s="71"/>
+      <c r="D97" s="68"/>
       <c r="E97" s="46"/>
       <c r="F97" s="31"/>
       <c r="G97" s="31"/>
@@ -8260,10 +8220,10 @@
       <c r="N97" s="31"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="73"/>
+      <c r="A98" s="71"/>
       <c r="B98" s="46"/>
       <c r="C98" s="31"/>
-      <c r="D98" s="71"/>
+      <c r="D98" s="68"/>
       <c r="E98" s="46"/>
       <c r="F98" s="31"/>
       <c r="G98" s="31"/>
@@ -8276,10 +8236,10 @@
       <c r="N98" s="31"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="73"/>
+      <c r="A99" s="71"/>
       <c r="B99" s="46"/>
       <c r="C99" s="31"/>
-      <c r="D99" s="71"/>
+      <c r="D99" s="68"/>
       <c r="E99" s="46"/>
       <c r="F99" s="31"/>
       <c r="G99" s="31"/>
@@ -8295,7 +8255,7 @@
       <c r="A100" s="73"/>
       <c r="B100" s="46"/>
       <c r="C100" s="31"/>
-      <c r="D100" s="71"/>
+      <c r="D100" s="68"/>
       <c r="E100" s="46"/>
       <c r="F100" s="31"/>
       <c r="G100" s="31"/>
@@ -8306,22 +8266,6 @@
       <c r="L100" s="31"/>
       <c r="M100" s="31"/>
       <c r="N100" s="31"/>
-    </row>
-    <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="74"/>
-      <c r="B101" s="46"/>
-      <c r="C101" s="31"/>
-      <c r="D101" s="71"/>
-      <c r="E101" s="46"/>
-      <c r="F101" s="31"/>
-      <c r="G101" s="31"/>
-      <c r="H101" s="31"/>
-      <c r="I101" s="31"/>
-      <c r="J101" s="31"/>
-      <c r="K101" s="31"/>
-      <c r="L101" s="31"/>
-      <c r="M101" s="31"/>
-      <c r="N101" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
CASEFLOW-4586 Update test spreadsheets with White RIver
</commit_message>
<xml_diff>
--- a/spec/support/allocationDuplicateRo.xlsx
+++ b/spec/support/allocationDuplicateRo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/spec/support/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremyshields/git-repos/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FA679B-D562-994E-9A30-708A48BACEFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD41AE64-4E53-2C47-9C57-4AACA734DE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20560" yWindow="460" windowWidth="17840" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RO Non-Availability Dates" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="129">
   <si>
     <t>Example</t>
   </si>
@@ -403,6 +403,12 @@
   </si>
   <si>
     <t>8:30</t>
+  </si>
+  <si>
+    <t>White River Junction, VT</t>
+  </si>
+  <si>
+    <t>RO05</t>
   </si>
 </sst>
 </file>
@@ -1208,41 +1214,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="10" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="10" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1268,6 +1243,37 @@
     <xf numFmtId="0" fontId="14" fillId="13" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="14" fillId="13" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="10" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="10" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2458,9 +2464,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IT50"/>
+  <dimension ref="A1:IU50"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2469,29 +2477,30 @@
     <col min="3" max="3" width="16.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="1" customWidth="1"/>
-    <col min="7" max="254" width="11" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="44" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="1" customWidth="1"/>
+    <col min="8" max="255" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:58" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="4"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
@@ -2534,9 +2543,10 @@
       <c r="BB1" s="4"/>
       <c r="BC1" s="4"/>
       <c r="BD1" s="4"/>
-      <c r="BE1" s="5"/>
-    </row>
-    <row r="2" spans="1:57" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE1" s="4"/>
+      <c r="BF1" s="5"/>
+    </row>
+    <row r="2" spans="1:58" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2553,163 +2563,166 @@
         <v>6</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="X2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="Y2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Z2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="AA2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="9" t="s">
+      <c r="AB2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="9" t="s">
+      <c r="AC2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AD2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AD2" s="9" t="s">
+      <c r="AE2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AE2" s="9" t="s">
+      <c r="AF2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AF2" s="9" t="s">
+      <c r="AG2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AG2" s="9" t="s">
+      <c r="AH2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AH2" s="9" t="s">
+      <c r="AI2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AI2" s="9" t="s">
+      <c r="AJ2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AJ2" s="9" t="s">
+      <c r="AK2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AK2" s="9" t="s">
+      <c r="AL2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AL2" s="9" t="s">
+      <c r="AM2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="AM2" s="9" t="s">
+      <c r="AN2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AN2" s="9" t="s">
+      <c r="AO2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="AO2" s="9" t="s">
+      <c r="AP2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="AP2" s="9" t="s">
+      <c r="AQ2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="AQ2" s="9" t="s">
+      <c r="AR2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AR2" s="9" t="s">
+      <c r="AS2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AS2" s="9" t="s">
+      <c r="AT2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AT2" s="9" t="s">
+      <c r="AU2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="AU2" s="9" t="s">
+      <c r="AV2" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="AV2" s="9" t="s">
+      <c r="AW2" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="AW2" s="9" t="s">
+      <c r="AX2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="AX2" s="9" t="s">
+      <c r="AY2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="AY2" s="9" t="s">
+      <c r="AZ2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AZ2" s="9" t="s">
+      <c r="BA2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="BA2" s="9" t="s">
+      <c r="BB2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="BB2" s="9" t="s">
+      <c r="BC2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="BC2" s="9" t="s">
+      <c r="BD2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="BD2" s="9" t="s">
+      <c r="BE2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="BE2" s="9" t="s">
+      <c r="BF2" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:57" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:58" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>59</v>
       </c>
@@ -2726,163 +2739,166 @@
         <v>63</v>
       </c>
       <c r="F3" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="N3" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="O3" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="P3" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="Q3" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="R3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="S3" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="T3" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="U3" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="V3" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="W3" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="W3" s="12" t="s">
+      <c r="X3" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="Y3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="Y3" s="12" t="s">
+      <c r="Z3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="Z3" s="12" t="s">
+      <c r="AA3" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AB3" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="AB3" s="12" t="s">
+      <c r="AC3" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="AC3" s="12" t="s">
+      <c r="AD3" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AD3" s="12" t="s">
+      <c r="AE3" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="AE3" s="12" t="s">
+      <c r="AF3" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="AF3" s="12" t="s">
+      <c r="AG3" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="AG3" s="12" t="s">
+      <c r="AH3" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="AH3" s="12" t="s">
+      <c r="AI3" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="AI3" s="12" t="s">
+      <c r="AJ3" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="AJ3" s="12" t="s">
+      <c r="AK3" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="AK3" s="12" t="s">
+      <c r="AL3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AL3" s="12" t="s">
+      <c r="AM3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="AM3" s="12" t="s">
+      <c r="AN3" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="AN3" s="12" t="s">
+      <c r="AO3" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="AO3" s="12" t="s">
+      <c r="AP3" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="AP3" s="12" t="s">
+      <c r="AQ3" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="AQ3" s="12" t="s">
+      <c r="AR3" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="AR3" s="12" t="s">
+      <c r="AS3" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="AS3" s="12" t="s">
+      <c r="AT3" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="AT3" s="12" t="s">
+      <c r="AU3" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="AU3" s="12" t="s">
+      <c r="AV3" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="AV3" s="12" t="s">
+      <c r="AW3" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="AW3" s="12" t="s">
+      <c r="AX3" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="AX3" s="12" t="s">
+      <c r="AY3" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="AY3" s="12" t="s">
+      <c r="AZ3" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="AZ3" s="12" t="s">
+      <c r="BA3" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="BA3" s="12" t="s">
+      <c r="BB3" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="BB3" s="12" t="s">
+      <c r="BC3" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="BC3" s="12" t="s">
+      <c r="BD3" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="BD3" s="12" t="s">
+      <c r="BE3" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="BE3" s="12" t="s">
+      <c r="BF3" s="12" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:57" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:58" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>116</v>
       </c>
@@ -3054,8 +3070,11 @@
       <c r="BE4" s="17">
         <v>43114</v>
       </c>
-    </row>
-    <row r="5" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF4" s="17">
+        <v>43114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18"/>
       <c r="B5" s="19">
         <v>43497</v>
@@ -3225,8 +3244,11 @@
       <c r="BE5" s="21">
         <v>43115</v>
       </c>
-    </row>
-    <row r="6" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF5" s="21">
+        <v>43115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18"/>
       <c r="B6" s="22">
         <v>43540</v>
@@ -3396,8 +3418,11 @@
       <c r="BE6" s="21">
         <v>43225</v>
       </c>
-    </row>
-    <row r="7" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF6" s="21">
+        <v>43225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18"/>
       <c r="B7" s="23">
         <v>43576</v>
@@ -3567,8 +3592,11 @@
       <c r="BE7" s="21">
         <v>43191</v>
       </c>
-    </row>
-    <row r="8" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF7" s="21">
+        <v>43191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18"/>
       <c r="B8" s="24">
         <v>43604</v>
@@ -3628,8 +3656,9 @@
       <c r="BC8" s="27"/>
       <c r="BD8" s="27"/>
       <c r="BE8" s="27"/>
-    </row>
-    <row r="9" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF8" s="27"/>
+    </row>
+    <row r="9" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18"/>
       <c r="B9" s="28"/>
       <c r="C9" s="29"/>
@@ -3687,8 +3716,9 @@
       <c r="BC9" s="27"/>
       <c r="BD9" s="27"/>
       <c r="BE9" s="27"/>
-    </row>
-    <row r="10" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF9" s="27"/>
+    </row>
+    <row r="10" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="18"/>
       <c r="B10" s="30"/>
       <c r="C10" s="31"/>
@@ -3746,8 +3776,9 @@
       <c r="BC10" s="26"/>
       <c r="BD10" s="26"/>
       <c r="BE10" s="26"/>
-    </row>
-    <row r="11" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF10" s="26"/>
+    </row>
+    <row r="11" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18"/>
       <c r="B11" s="32"/>
       <c r="C11" s="29"/>
@@ -3804,9 +3835,10 @@
       <c r="BB11" s="29"/>
       <c r="BC11" s="29"/>
       <c r="BD11" s="29"/>
-      <c r="BE11" s="33"/>
-    </row>
-    <row r="12" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE11" s="29"/>
+      <c r="BF11" s="33"/>
+    </row>
+    <row r="12" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18"/>
       <c r="B12" s="30"/>
       <c r="C12" s="31"/>
@@ -3864,8 +3896,9 @@
       <c r="BC12" s="31"/>
       <c r="BD12" s="31"/>
       <c r="BE12" s="31"/>
-    </row>
-    <row r="13" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF12" s="31"/>
+    </row>
+    <row r="13" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18"/>
       <c r="B13" s="32"/>
       <c r="C13" s="29"/>
@@ -3922,9 +3955,10 @@
       <c r="BB13" s="29"/>
       <c r="BC13" s="29"/>
       <c r="BD13" s="29"/>
-      <c r="BE13" s="33"/>
-    </row>
-    <row r="14" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE13" s="29"/>
+      <c r="BF13" s="33"/>
+    </row>
+    <row r="14" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18"/>
       <c r="B14" s="30"/>
       <c r="C14" s="31"/>
@@ -3982,8 +4016,9 @@
       <c r="BC14" s="31"/>
       <c r="BD14" s="31"/>
       <c r="BE14" s="31"/>
-    </row>
-    <row r="15" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF14" s="31"/>
+    </row>
+    <row r="15" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
       <c r="B15" s="32"/>
       <c r="C15" s="29"/>
@@ -4040,9 +4075,10 @@
       <c r="BB15" s="29"/>
       <c r="BC15" s="29"/>
       <c r="BD15" s="29"/>
-      <c r="BE15" s="33"/>
-    </row>
-    <row r="16" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE15" s="29"/>
+      <c r="BF15" s="33"/>
+    </row>
+    <row r="16" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
       <c r="B16" s="30"/>
       <c r="C16" s="31"/>
@@ -4100,8 +4136,9 @@
       <c r="BC16" s="31"/>
       <c r="BD16" s="31"/>
       <c r="BE16" s="31"/>
-    </row>
-    <row r="17" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF16" s="31"/>
+    </row>
+    <row r="17" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
       <c r="B17" s="32"/>
       <c r="C17" s="29"/>
@@ -4158,9 +4195,10 @@
       <c r="BB17" s="29"/>
       <c r="BC17" s="29"/>
       <c r="BD17" s="29"/>
-      <c r="BE17" s="33"/>
-    </row>
-    <row r="18" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE17" s="29"/>
+      <c r="BF17" s="33"/>
+    </row>
+    <row r="18" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18"/>
       <c r="B18" s="30"/>
       <c r="C18" s="31"/>
@@ -4218,8 +4256,9 @@
       <c r="BC18" s="31"/>
       <c r="BD18" s="31"/>
       <c r="BE18" s="31"/>
-    </row>
-    <row r="19" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF18" s="31"/>
+    </row>
+    <row r="19" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18"/>
       <c r="B19" s="32"/>
       <c r="C19" s="29"/>
@@ -4276,9 +4315,10 @@
       <c r="BB19" s="29"/>
       <c r="BC19" s="29"/>
       <c r="BD19" s="29"/>
-      <c r="BE19" s="33"/>
-    </row>
-    <row r="20" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE19" s="29"/>
+      <c r="BF19" s="33"/>
+    </row>
+    <row r="20" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18"/>
       <c r="B20" s="30"/>
       <c r="C20" s="31"/>
@@ -4336,8 +4376,9 @@
       <c r="BC20" s="31"/>
       <c r="BD20" s="31"/>
       <c r="BE20" s="31"/>
-    </row>
-    <row r="21" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF20" s="31"/>
+    </row>
+    <row r="21" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
       <c r="B21" s="32"/>
       <c r="C21" s="29"/>
@@ -4394,9 +4435,10 @@
       <c r="BB21" s="29"/>
       <c r="BC21" s="29"/>
       <c r="BD21" s="29"/>
-      <c r="BE21" s="33"/>
-    </row>
-    <row r="22" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE21" s="29"/>
+      <c r="BF21" s="33"/>
+    </row>
+    <row r="22" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
       <c r="B22" s="30"/>
       <c r="C22" s="31"/>
@@ -4454,8 +4496,9 @@
       <c r="BC22" s="31"/>
       <c r="BD22" s="31"/>
       <c r="BE22" s="31"/>
-    </row>
-    <row r="23" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF22" s="31"/>
+    </row>
+    <row r="23" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
       <c r="B23" s="32"/>
       <c r="C23" s="29"/>
@@ -4512,9 +4555,10 @@
       <c r="BB23" s="29"/>
       <c r="BC23" s="29"/>
       <c r="BD23" s="29"/>
-      <c r="BE23" s="33"/>
-    </row>
-    <row r="24" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE23" s="29"/>
+      <c r="BF23" s="33"/>
+    </row>
+    <row r="24" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18"/>
       <c r="B24" s="30"/>
       <c r="C24" s="31"/>
@@ -4572,8 +4616,9 @@
       <c r="BC24" s="31"/>
       <c r="BD24" s="31"/>
       <c r="BE24" s="31"/>
-    </row>
-    <row r="25" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF24" s="31"/>
+    </row>
+    <row r="25" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18"/>
       <c r="B25" s="32"/>
       <c r="C25" s="29"/>
@@ -4630,9 +4675,10 @@
       <c r="BB25" s="29"/>
       <c r="BC25" s="29"/>
       <c r="BD25" s="29"/>
-      <c r="BE25" s="33"/>
-    </row>
-    <row r="26" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE25" s="29"/>
+      <c r="BF25" s="33"/>
+    </row>
+    <row r="26" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="18"/>
       <c r="B26" s="30"/>
       <c r="C26" s="31"/>
@@ -4690,8 +4736,9 @@
       <c r="BC26" s="31"/>
       <c r="BD26" s="31"/>
       <c r="BE26" s="31"/>
-    </row>
-    <row r="27" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF26" s="31"/>
+    </row>
+    <row r="27" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18"/>
       <c r="B27" s="32"/>
       <c r="C27" s="29"/>
@@ -4748,9 +4795,10 @@
       <c r="BB27" s="29"/>
       <c r="BC27" s="29"/>
       <c r="BD27" s="29"/>
-      <c r="BE27" s="33"/>
-    </row>
-    <row r="28" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE27" s="29"/>
+      <c r="BF27" s="33"/>
+    </row>
+    <row r="28" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18"/>
       <c r="B28" s="30"/>
       <c r="C28" s="31"/>
@@ -4808,8 +4856,9 @@
       <c r="BC28" s="31"/>
       <c r="BD28" s="31"/>
       <c r="BE28" s="31"/>
-    </row>
-    <row r="29" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF28" s="31"/>
+    </row>
+    <row r="29" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="18"/>
       <c r="B29" s="32"/>
       <c r="C29" s="29"/>
@@ -4866,9 +4915,10 @@
       <c r="BB29" s="29"/>
       <c r="BC29" s="29"/>
       <c r="BD29" s="29"/>
-      <c r="BE29" s="33"/>
-    </row>
-    <row r="30" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE29" s="29"/>
+      <c r="BF29" s="33"/>
+    </row>
+    <row r="30" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="18"/>
       <c r="B30" s="30"/>
       <c r="C30" s="31"/>
@@ -4926,8 +4976,9 @@
       <c r="BC30" s="31"/>
       <c r="BD30" s="31"/>
       <c r="BE30" s="31"/>
-    </row>
-    <row r="31" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF30" s="31"/>
+    </row>
+    <row r="31" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="18"/>
       <c r="B31" s="32"/>
       <c r="C31" s="29"/>
@@ -4984,9 +5035,10 @@
       <c r="BB31" s="29"/>
       <c r="BC31" s="29"/>
       <c r="BD31" s="29"/>
-      <c r="BE31" s="33"/>
-    </row>
-    <row r="32" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE31" s="29"/>
+      <c r="BF31" s="33"/>
+    </row>
+    <row r="32" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="18"/>
       <c r="B32" s="30"/>
       <c r="C32" s="31"/>
@@ -5044,8 +5096,9 @@
       <c r="BC32" s="31"/>
       <c r="BD32" s="31"/>
       <c r="BE32" s="31"/>
-    </row>
-    <row r="33" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF32" s="31"/>
+    </row>
+    <row r="33" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="18"/>
       <c r="B33" s="32"/>
       <c r="C33" s="29"/>
@@ -5102,9 +5155,10 @@
       <c r="BB33" s="29"/>
       <c r="BC33" s="29"/>
       <c r="BD33" s="29"/>
-      <c r="BE33" s="33"/>
-    </row>
-    <row r="34" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE33" s="29"/>
+      <c r="BF33" s="33"/>
+    </row>
+    <row r="34" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18"/>
       <c r="B34" s="30"/>
       <c r="C34" s="31"/>
@@ -5162,8 +5216,9 @@
       <c r="BC34" s="31"/>
       <c r="BD34" s="31"/>
       <c r="BE34" s="31"/>
-    </row>
-    <row r="35" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF34" s="31"/>
+    </row>
+    <row r="35" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="18"/>
       <c r="B35" s="32"/>
       <c r="C35" s="29"/>
@@ -5220,9 +5275,10 @@
       <c r="BB35" s="29"/>
       <c r="BC35" s="29"/>
       <c r="BD35" s="29"/>
-      <c r="BE35" s="33"/>
-    </row>
-    <row r="36" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE35" s="29"/>
+      <c r="BF35" s="33"/>
+    </row>
+    <row r="36" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="18"/>
       <c r="B36" s="30"/>
       <c r="C36" s="31"/>
@@ -5280,8 +5336,9 @@
       <c r="BC36" s="31"/>
       <c r="BD36" s="31"/>
       <c r="BE36" s="31"/>
-    </row>
-    <row r="37" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF36" s="31"/>
+    </row>
+    <row r="37" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="18"/>
       <c r="B37" s="32"/>
       <c r="C37" s="29"/>
@@ -5338,9 +5395,10 @@
       <c r="BB37" s="29"/>
       <c r="BC37" s="29"/>
       <c r="BD37" s="29"/>
-      <c r="BE37" s="33"/>
-    </row>
-    <row r="38" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE37" s="29"/>
+      <c r="BF37" s="33"/>
+    </row>
+    <row r="38" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="18"/>
       <c r="B38" s="30"/>
       <c r="C38" s="31"/>
@@ -5398,8 +5456,9 @@
       <c r="BC38" s="31"/>
       <c r="BD38" s="31"/>
       <c r="BE38" s="31"/>
-    </row>
-    <row r="39" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF38" s="31"/>
+    </row>
+    <row r="39" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="18"/>
       <c r="B39" s="32"/>
       <c r="C39" s="29"/>
@@ -5456,9 +5515,10 @@
       <c r="BB39" s="29"/>
       <c r="BC39" s="29"/>
       <c r="BD39" s="29"/>
-      <c r="BE39" s="33"/>
-    </row>
-    <row r="40" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE39" s="29"/>
+      <c r="BF39" s="33"/>
+    </row>
+    <row r="40" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="18"/>
       <c r="B40" s="30"/>
       <c r="C40" s="31"/>
@@ -5516,8 +5576,9 @@
       <c r="BC40" s="31"/>
       <c r="BD40" s="31"/>
       <c r="BE40" s="31"/>
-    </row>
-    <row r="41" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF40" s="31"/>
+    </row>
+    <row r="41" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="18"/>
       <c r="B41" s="32"/>
       <c r="C41" s="29"/>
@@ -5574,9 +5635,10 @@
       <c r="BB41" s="29"/>
       <c r="BC41" s="29"/>
       <c r="BD41" s="29"/>
-      <c r="BE41" s="33"/>
-    </row>
-    <row r="42" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE41" s="29"/>
+      <c r="BF41" s="33"/>
+    </row>
+    <row r="42" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="18"/>
       <c r="B42" s="30"/>
       <c r="C42" s="31"/>
@@ -5634,8 +5696,9 @@
       <c r="BC42" s="31"/>
       <c r="BD42" s="31"/>
       <c r="BE42" s="31"/>
-    </row>
-    <row r="43" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF42" s="31"/>
+    </row>
+    <row r="43" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="18"/>
       <c r="B43" s="32"/>
       <c r="C43" s="29"/>
@@ -5692,9 +5755,10 @@
       <c r="BB43" s="29"/>
       <c r="BC43" s="29"/>
       <c r="BD43" s="29"/>
-      <c r="BE43" s="33"/>
-    </row>
-    <row r="44" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE43" s="29"/>
+      <c r="BF43" s="33"/>
+    </row>
+    <row r="44" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="18"/>
       <c r="B44" s="30"/>
       <c r="C44" s="31"/>
@@ -5752,8 +5816,9 @@
       <c r="BC44" s="31"/>
       <c r="BD44" s="31"/>
       <c r="BE44" s="31"/>
-    </row>
-    <row r="45" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF44" s="31"/>
+    </row>
+    <row r="45" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="18"/>
       <c r="B45" s="32"/>
       <c r="C45" s="29"/>
@@ -5810,9 +5875,10 @@
       <c r="BB45" s="29"/>
       <c r="BC45" s="29"/>
       <c r="BD45" s="29"/>
-      <c r="BE45" s="33"/>
-    </row>
-    <row r="46" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE45" s="29"/>
+      <c r="BF45" s="33"/>
+    </row>
+    <row r="46" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="18"/>
       <c r="B46" s="30"/>
       <c r="C46" s="31"/>
@@ -5870,8 +5936,9 @@
       <c r="BC46" s="31"/>
       <c r="BD46" s="31"/>
       <c r="BE46" s="31"/>
-    </row>
-    <row r="47" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF46" s="31"/>
+    </row>
+    <row r="47" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="18"/>
       <c r="B47" s="32"/>
       <c r="C47" s="29"/>
@@ -5928,9 +5995,10 @@
       <c r="BB47" s="29"/>
       <c r="BC47" s="29"/>
       <c r="BD47" s="29"/>
-      <c r="BE47" s="33"/>
-    </row>
-    <row r="48" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE47" s="29"/>
+      <c r="BF47" s="33"/>
+    </row>
+    <row r="48" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="18"/>
       <c r="B48" s="30"/>
       <c r="C48" s="31"/>
@@ -5988,8 +6056,9 @@
       <c r="BC48" s="31"/>
       <c r="BD48" s="31"/>
       <c r="BE48" s="31"/>
-    </row>
-    <row r="49" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BF48" s="31"/>
+    </row>
+    <row r="49" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="18"/>
       <c r="B49" s="32"/>
       <c r="C49" s="29"/>
@@ -6046,9 +6115,10 @@
       <c r="BB49" s="29"/>
       <c r="BC49" s="29"/>
       <c r="BD49" s="29"/>
-      <c r="BE49" s="33"/>
-    </row>
-    <row r="50" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BE49" s="29"/>
+      <c r="BF49" s="33"/>
+    </row>
+    <row r="50" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="34"/>
       <c r="B50" s="35"/>
       <c r="C50" s="36"/>
@@ -6106,10 +6176,11 @@
       <c r="BC50" s="36"/>
       <c r="BD50" s="36"/>
       <c r="BE50" s="36"/>
+      <c r="BF50" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="C1:N1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -6135,10 +6206,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="59"/>
+      <c r="B1" s="72"/>
       <c r="C1" s="38"/>
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
@@ -6234,10 +6305,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:IV99"/>
+  <dimension ref="A1:IV100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6251,16 +6322,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="73" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="62"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="75"/>
       <c r="I1" s="45"/>
       <c r="J1" s="45"/>
       <c r="K1" s="45"/>
@@ -6269,16 +6340,16 @@
       <c r="N1" s="45"/>
     </row>
     <row r="2" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="63"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="65" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="67"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="78"/>
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
       <c r="K2" s="27"/>
@@ -6287,26 +6358,26 @@
       <c r="N2" s="27"/>
     </row>
     <row r="3" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="68"/>
-      <c r="B3" s="69" t="s">
+      <c r="A3" s="57"/>
+      <c r="B3" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="71" t="s">
+      <c r="E3" s="60" t="s">
         <v>122</v>
       </c>
-      <c r="F3" s="72" t="s">
+      <c r="F3" s="61" t="s">
         <v>123</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="60" t="s">
         <v>124</v>
       </c>
-      <c r="H3" s="71" t="s">
+      <c r="H3" s="60" t="s">
         <v>125</v>
       </c>
       <c r="I3" s="27"/>
@@ -6317,28 +6388,28 @@
       <c r="N3" s="27"/>
     </row>
     <row r="4" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="74" t="s">
+      <c r="A4" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="76">
+      <c r="D4" s="65">
         <v>10</v>
       </c>
-      <c r="E4" s="77">
+      <c r="E4" s="66">
         <v>50</v>
       </c>
-      <c r="F4" s="77">
+      <c r="F4" s="66">
         <v>8</v>
       </c>
-      <c r="G4" s="77">
+      <c r="G4" s="66">
         <v>60</v>
       </c>
-      <c r="H4" s="78" t="s">
+      <c r="H4" s="67" t="s">
         <v>126</v>
       </c>
       <c r="I4" s="27"/>
@@ -6471,13 +6542,13 @@
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="52"/>
       <c r="B9" s="47" t="s">
-        <v>64</v>
+        <v>127</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="D9" s="49">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E9" s="38">
         <v>0</v>
@@ -6501,13 +6572,13 @@
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="52"/>
       <c r="B10" s="47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="49">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E10" s="38">
         <v>0</v>
@@ -6531,13 +6602,13 @@
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="52"/>
       <c r="B11" s="47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="49">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E11" s="38">
         <v>0</v>
@@ -6561,13 +6632,13 @@
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="52"/>
       <c r="B12" s="47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="49">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E12" s="38">
         <v>0</v>
@@ -6591,13 +6662,13 @@
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="52"/>
       <c r="B13" s="47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="49">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E13" s="38">
         <v>0</v>
@@ -6621,13 +6692,13 @@
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="52"/>
       <c r="B14" s="47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="49">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E14" s="38">
         <v>0</v>
@@ -6651,13 +6722,13 @@
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="52"/>
       <c r="B15" s="47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="49">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="38">
         <v>0</v>
@@ -6681,13 +6752,13 @@
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="52"/>
       <c r="B16" s="47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" s="49">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E16" s="38">
         <v>0</v>
@@ -6711,13 +6782,13 @@
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="52"/>
       <c r="B17" s="47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E17" s="38">
         <v>0</v>
@@ -6741,13 +6812,13 @@
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="52"/>
       <c r="B18" s="47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="49">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E18" s="38">
         <v>0</v>
@@ -6771,13 +6842,13 @@
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="52"/>
       <c r="B19" s="47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="49">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E19" s="38">
         <v>0</v>
@@ -6801,13 +6872,13 @@
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="52"/>
       <c r="B20" s="47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="49">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E20" s="38">
         <v>0</v>
@@ -6831,13 +6902,13 @@
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="52"/>
       <c r="B21" s="47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" s="49">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E21" s="38">
         <v>0</v>
@@ -6861,13 +6932,13 @@
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="52"/>
       <c r="B22" s="47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="49">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E22" s="38">
         <v>0</v>
@@ -6891,13 +6962,13 @@
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="52"/>
       <c r="B23" s="47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" s="49">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E23" s="38">
         <v>0</v>
@@ -6921,13 +6992,13 @@
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="52"/>
       <c r="B24" s="47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D24" s="49">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E24" s="38">
         <v>0</v>
@@ -6951,13 +7022,13 @@
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="52"/>
       <c r="B25" s="47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D25" s="49">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E25" s="38">
         <v>0</v>
@@ -6981,13 +7052,13 @@
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="52"/>
       <c r="B26" s="47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" s="49">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E26" s="38">
         <v>0</v>
@@ -7011,13 +7082,13 @@
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="52"/>
       <c r="B27" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D27" s="49">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E27" s="38">
         <v>0</v>
@@ -7041,13 +7112,13 @@
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="52"/>
       <c r="B28" s="47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D28" s="49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E28" s="38">
         <v>0</v>
@@ -7071,13 +7142,13 @@
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="52"/>
       <c r="B29" s="47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29" s="48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" s="49">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E29" s="38">
         <v>0</v>
@@ -7101,13 +7172,13 @@
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="52"/>
       <c r="B30" s="47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D30" s="49">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E30" s="38">
         <v>0</v>
@@ -7131,13 +7202,13 @@
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="52"/>
       <c r="B31" s="47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D31" s="49">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E31" s="38">
         <v>0</v>
@@ -7161,10 +7232,10 @@
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="52"/>
       <c r="B32" s="47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C32" s="48" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" s="49">
         <v>4</v>
@@ -7191,13 +7262,13 @@
     <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="52"/>
       <c r="B33" s="47" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="C33" s="48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" s="49">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E33" s="38">
         <v>0</v>
@@ -7221,13 +7292,13 @@
     <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="52"/>
       <c r="B34" s="47" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="C34" s="48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" s="49">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E34" s="38">
         <v>0</v>
@@ -7251,13 +7322,13 @@
     <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="52"/>
       <c r="B35" s="47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C35" s="48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D35" s="49">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E35" s="38">
         <v>0</v>
@@ -7281,13 +7352,13 @@
     <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="52"/>
       <c r="B36" s="47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" s="48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" s="49">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E36" s="38">
         <v>0</v>
@@ -7311,13 +7382,13 @@
     <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="52"/>
       <c r="B37" s="47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C37" s="48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" s="49">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E37" s="38">
         <v>0</v>
@@ -7341,13 +7412,13 @@
     <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="52"/>
       <c r="B38" s="47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C38" s="48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D38" s="49">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E38" s="38">
         <v>0</v>
@@ -7371,13 +7442,13 @@
     <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="52"/>
       <c r="B39" s="47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C39" s="48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D39" s="49">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E39" s="38">
         <v>0</v>
@@ -7401,13 +7472,13 @@
     <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="52"/>
       <c r="B40" s="47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C40" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D40" s="49">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E40" s="38">
         <v>0</v>
@@ -7431,13 +7502,13 @@
     <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="52"/>
       <c r="B41" s="47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C41" s="48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D41" s="49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E41" s="38">
         <v>0</v>
@@ -7461,13 +7532,13 @@
     <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="52"/>
       <c r="B42" s="47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C42" s="48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D42" s="49">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E42" s="38">
         <v>0</v>
@@ -7491,13 +7562,13 @@
     <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="52"/>
       <c r="B43" s="47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C43" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D43" s="49">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E43" s="38">
         <v>0</v>
@@ -7521,13 +7592,13 @@
     <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="52"/>
       <c r="B44" s="47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C44" s="48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D44" s="49">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E44" s="38">
         <v>0</v>
@@ -7551,13 +7622,13 @@
     <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="52"/>
       <c r="B45" s="47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C45" s="48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D45" s="49">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E45" s="38">
         <v>0</v>
@@ -7581,13 +7652,13 @@
     <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="52"/>
       <c r="B46" s="47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C46" s="48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D46" s="49">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="E46" s="38">
         <v>0</v>
@@ -7611,13 +7682,13 @@
     <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="52"/>
       <c r="B47" s="47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C47" s="48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D47" s="49">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="E47" s="38">
         <v>0</v>
@@ -7641,13 +7712,13 @@
     <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="52"/>
       <c r="B48" s="47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C48" s="48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D48" s="49">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E48" s="38">
         <v>0</v>
@@ -7671,13 +7742,13 @@
     <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="52"/>
       <c r="B49" s="47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C49" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D49" s="49">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E49" s="38">
         <v>0</v>
@@ -7701,13 +7772,13 @@
     <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="52"/>
       <c r="B50" s="47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C50" s="48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D50" s="49">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="E50" s="38">
         <v>0</v>
@@ -7731,13 +7802,13 @@
     <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="52"/>
       <c r="B51" s="47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C51" s="48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D51" s="49">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="E51" s="38">
         <v>0</v>
@@ -7761,13 +7832,13 @@
     <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="52"/>
       <c r="B52" s="47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C52" s="48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D52" s="49">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E52" s="38">
         <v>0</v>
@@ -7791,13 +7862,13 @@
     <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="52"/>
       <c r="B53" s="47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C53" s="48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D53" s="49">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E53" s="38">
         <v>0</v>
@@ -7821,13 +7892,13 @@
     <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="52"/>
       <c r="B54" s="47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C54" s="48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D54" s="49">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E54" s="38">
         <v>0</v>
@@ -7851,13 +7922,13 @@
     <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="52"/>
       <c r="B55" s="47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C55" s="48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D55" s="49">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E55" s="38">
         <v>0</v>
@@ -7881,13 +7952,13 @@
     <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="52"/>
       <c r="B56" s="47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C56" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D56" s="49">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E56" s="38">
         <v>0</v>
@@ -7911,13 +7982,13 @@
     <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="52"/>
       <c r="B57" s="47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C57" s="48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D57" s="49">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E57" s="38">
         <v>0</v>
@@ -7941,10 +8012,10 @@
     <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="52"/>
       <c r="B58" s="47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C58" s="48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D58" s="49">
         <v>2</v>
@@ -7971,13 +8042,13 @@
     <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="52"/>
       <c r="B59" s="47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C59" s="48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D59" s="49">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E59" s="38">
         <v>0</v>
@@ -8001,13 +8072,13 @@
     <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="52"/>
       <c r="B60" s="47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C60" s="48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D60" s="49">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E60" s="38">
         <v>0</v>
@@ -8030,13 +8101,27 @@
     </row>
     <row r="61" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="52"/>
-      <c r="B61" s="53"/>
-      <c r="C61" s="27"/>
-      <c r="D61" s="49"/>
-      <c r="E61" s="38"/>
-      <c r="F61" s="27"/>
-      <c r="G61" s="27"/>
-      <c r="H61" s="27"/>
+      <c r="B61" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="C61" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="D61" s="49">
+        <v>1</v>
+      </c>
+      <c r="E61" s="38">
+        <v>0</v>
+      </c>
+      <c r="F61" s="27">
+        <v>0</v>
+      </c>
+      <c r="G61" s="27">
+        <v>0</v>
+      </c>
+      <c r="H61" s="27">
+        <v>0</v>
+      </c>
       <c r="I61" s="27"/>
       <c r="J61" s="27"/>
       <c r="K61" s="27"/>
@@ -8046,7 +8131,7 @@
     </row>
     <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="52"/>
-      <c r="B62" s="38"/>
+      <c r="B62" s="53"/>
       <c r="C62" s="27"/>
       <c r="D62" s="49"/>
       <c r="E62" s="38"/>
@@ -8637,7 +8722,7 @@
       <c r="N98" s="27"/>
     </row>
     <row r="99" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="54"/>
+      <c r="A99" s="52"/>
       <c r="B99" s="38"/>
       <c r="C99" s="27"/>
       <c r="D99" s="49"/>
@@ -8652,6 +8737,22 @@
       <c r="M99" s="27"/>
       <c r="N99" s="27"/>
     </row>
+    <row r="100" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="54"/>
+      <c r="B100" s="38"/>
+      <c r="C100" s="27"/>
+      <c r="D100" s="49"/>
+      <c r="E100" s="38"/>
+      <c r="F100" s="27"/>
+      <c r="G100" s="27"/>
+      <c r="H100" s="27"/>
+      <c r="I100" s="27"/>
+      <c r="J100" s="27"/>
+      <c r="K100" s="27"/>
+      <c r="L100" s="27"/>
+      <c r="M100" s="27"/>
+      <c r="N100" s="27"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>

</xml_diff>

<commit_message>
CASEFLOW-4586 test spread sheet fixes
</commit_message>
<xml_diff>
--- a/spec/support/allocationDuplicateRo.xlsx
+++ b/spec/support/allocationDuplicateRo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremyshields/git-repos/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44AFEC2-F196-AE45-9935-44C077206C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2905273F-7BE6-EE45-A205-4C3BC0EACC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6308,7 +6308,7 @@
   <dimension ref="A1:IV100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6548,7 +6548,7 @@
         <v>128</v>
       </c>
       <c r="D9" s="49">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E9" s="38">
         <v>0</v>

</xml_diff>